<commit_message>
banner del blog v2, loading imgs
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD299FB-8E5E-4076-8131-192D3F2B0436}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA0EF9B-2058-4F89-9061-BABFF7FD9143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="230">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -951,6 +951,12 @@
   </si>
   <si>
     <t>no sabia como avarcar el desafio de como crear un diseño yo mismo, prove varios metodos hasta que me decidi por este</t>
+  </si>
+  <si>
+    <t>cree un diseño un poco mejor, cambie la vercion de movil y la de pc, ademas de esto agrege un efecto de loading mas optimizado para telefonos y para computadoras, ademas las imágenes antes se aplantaban cuando no cargaban ahora las imágenes adoptan un tamaño previo y al cargar la imagen ahi si ocupa el espacio que le coresponde, la funcion de cargar tambien la agrege a los frames (osea a los pdfs)</t>
+  </si>
+  <si>
+    <t>sin dificultades</t>
   </si>
 </sst>
 </file>
@@ -2806,6 +2812,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2839,18 +2938,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2860,85 +2947,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2959,12 +3040,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2977,74 +3052,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3057,96 +3153,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4133,56 +4139,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4194,45 +4200,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4243,84 +4249,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4329,10 +4335,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4342,8 +4348,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4352,8 +4358,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4362,8 +4368,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4372,8 +4378,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4382,10 +4388,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4396,10 +4402,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4410,8 +4416,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4420,10 +4426,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4434,8 +4440,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4444,8 +4450,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4454,8 +4460,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4464,8 +4470,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4474,8 +4480,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4484,8 +4490,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4494,8 +4500,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4504,8 +4510,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4514,8 +4520,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4524,8 +4530,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4534,10 +4540,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4548,8 +4554,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4558,8 +4564,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4568,8 +4574,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4578,10 +4584,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4592,8 +4598,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4602,10 +4608,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4616,10 +4622,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4630,10 +4636,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4644,8 +4650,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4654,8 +4660,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4664,8 +4670,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4674,8 +4680,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4684,8 +4690,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4694,10 +4700,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4715,44 +4721,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4769,6 +4737,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4784,7 +4790,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,14 +4872,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4895,14 +4901,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4924,14 +4930,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4953,14 +4959,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4982,14 +4988,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5185,16 +5191,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5266,20 +5272,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>8</v>
       </c>
-      <c r="F17" s="228" t="s">
+      <c r="F17" s="224" t="s">
         <v>221</v>
       </c>
-      <c r="G17" s="229"/>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5347,20 +5353,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5402,14 +5408,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5434,17 +5440,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5588,10 +5594,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5618,8 +5624,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -6123,12 +6129,22 @@
       <c r="Y44" s="18"/>
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="216"/>
+      <c r="B45" s="216" t="s">
+        <v>228</v>
+      </c>
       <c r="C45" s="217"/>
-      <c r="D45" s="161"/>
-      <c r="E45" s="161"/>
-      <c r="F45" s="160"/>
-      <c r="G45" s="160"/>
+      <c r="D45" s="161">
+        <v>45755</v>
+      </c>
+      <c r="E45" s="161">
+        <v>45755</v>
+      </c>
+      <c r="F45" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G45" s="160" t="s">
+        <v>229</v>
+      </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
       <c r="J45" s="18"/>
@@ -6507,14 +6523,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6773,9 +6789,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6800,11 +6816,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6829,10 +6845,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6855,11 +6871,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6911,11 +6927,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6937,11 +6953,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6968,10 +6984,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7049,14 +7065,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7078,14 +7094,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7116,22 +7132,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7148,14 +7156,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7272,124 +7288,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7418,66 +7434,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7506,66 +7522,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7594,66 +7610,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7682,184 +7698,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7874,13 +7878,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
tamaños de imagenes, pagina directorio
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA0EF9B-2058-4F89-9061-BABFF7FD9143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC38DD3D-97AC-4F92-BFE3-364A9B7CC61F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="229">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,14 +874,6 @@
     <t>falle muchas veces intentando ver la forma en que poder agregar secciones y variables compatibles con el editor de blogger</t>
   </si>
   <si>
-    <t>agrege animaciones ala oprimir las imágenes y al pasar el mause sobre el boton de descarga, ahora el menu izquierdo se queda fijado a la derecha aun que el main no tenga contenido
-antes las estaditicas al aparecer lo haciena repentinamente moviendo todo el menu asi abajo, ahora tiene su porpio espasio antes de aparecer tons no hara ese salto, ademas que ahora aparece con un lindo difuminado, la grafica de blogger la decore y ahora se puede habilitar desde el menu de bogger, ademas esta tambien cuenta con una animacion ala parecer</t>
-  </si>
-  <si>
-    <t>seme complico vastante la forma en la que funciona la grafica me tomo un buen tiempo poder posisionarla bien 
-ademas de esto estaba intentado hacer su diseño gris pero seme fue imposible, lo intente pero nada, esto dibido a que no fui capaz de usar la variable que manejaba este estado</t>
-  </si>
-  <si>
     <t>comenze con el modelado en html de una skleton loader, investigue aserca de elllos y hise mi vercion para la pagina wep,  despues lo implemente, y aparecera mientras hayan recursos cargando, aun que… no se si valga la pena ya que le añade html inesesario a la pagina
 ademas de esto estuve intentado solucionar el problema del mal posisiconamiento de los whigests en blogger, identifique el problema, eso es dibido al estilo flex que se le aplica, desafortunadamente aun no lo eh solucionado, todas mis ideas an fracasado, seguire intentando mañana</t>
   </si>
@@ -957,6 +949,14 @@
   </si>
   <si>
     <t>sin dificultades</t>
+  </si>
+  <si>
+    <t>hise que las imágenes estuvieran bien centradas cuando no gargan en pc
+esta experimientando con poder posicionar las imgenes según la alineacion del texto en el editor de contenido de blogger pero esto me daba errores en el blog principal y luego de un rato con intentando hacer que ambas cosas funcionaran a la vez decidi rendirme
+el punto anterior lo aproveche para organizar un poco mejor esa parte del css ademas mover algunas cosillas como por ejemplo ahora el tamaño es totalmente personalizables y se puden crear cuadriculas 
+ya no se generan la cuadriculas automaticamente para dar mas liverdad de personalizacion
+antes las imagenes se descargaban en poca calidad, lo cambie ahora ya se descargabn con buena resolucion
+inplemente la pagina del directorio del centro, edite la imagen con la lista yo mismo con mi experiencia en edicion de imagenes</t>
   </si>
 </sst>
 </file>
@@ -2812,6 +2812,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2824,6 +2857,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2875,77 +2947,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2965,99 +3052,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3076,83 +3151,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4139,56 +4139,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4200,45 +4200,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4249,84 +4249,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4335,10 +4335,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4348,8 +4348,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4358,8 +4358,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4368,8 +4368,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4378,8 +4378,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4388,10 +4388,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4402,10 +4402,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4416,8 +4416,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4426,10 +4426,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4440,8 +4440,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4450,8 +4450,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4460,8 +4460,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4470,8 +4470,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4480,8 +4480,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4490,8 +4490,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4500,8 +4500,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4510,8 +4510,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4520,8 +4520,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4530,8 +4530,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4540,10 +4540,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4554,8 +4554,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4564,8 +4564,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4574,8 +4574,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4584,10 +4584,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4598,8 +4598,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4608,10 +4608,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4622,10 +4622,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4636,10 +4636,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4650,8 +4650,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4660,8 +4660,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4670,8 +4670,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4680,8 +4680,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4690,8 +4690,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4700,10 +4700,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4721,6 +4721,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4737,44 +4775,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4790,7 +4790,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4872,14 +4872,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4901,14 +4901,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4930,14 +4930,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4959,14 +4959,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4988,14 +4988,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5191,16 +5191,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5272,20 +5272,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>8</v>
       </c>
-      <c r="F17" s="224" t="s">
-        <v>221</v>
-      </c>
-      <c r="G17" s="225"/>
+      <c r="F17" s="228" t="s">
+        <v>219</v>
+      </c>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5353,20 +5353,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5408,14 +5408,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5440,17 +5440,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5594,10 +5594,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5624,8 +5624,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="40" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="216" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C40" s="217"/>
       <c r="D40" s="161">
@@ -5977,7 +5977,7 @@
         <v>204</v>
       </c>
       <c r="G40" s="160" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
@@ -6000,7 +6000,7 @@
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6013,7 +6013,7 @@
         <v>204</v>
       </c>
       <c r="G41" s="160" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
@@ -6094,7 +6094,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6107,7 +6107,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6130,7 +6130,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6143,7 +6143,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6166,20 +6166,20 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
-        <v>45741</v>
+        <v>45756</v>
       </c>
       <c r="E46" s="161">
-        <v>45741</v>
+        <v>45756</v>
       </c>
       <c r="F46" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G46" s="160" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6215,7 +6215,7 @@
         <v>204</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6238,7 +6238,7 @@
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="216" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C48" s="217"/>
       <c r="D48" s="161">
@@ -6251,7 +6251,7 @@
         <v>204</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6274,7 +6274,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6287,7 +6287,7 @@
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6362,7 +6362,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6375,7 +6375,7 @@
         <v>204</v>
       </c>
       <c r="G52" s="160" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H52" s="20"/>
       <c r="I52" s="18"/>
@@ -6398,7 +6398,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
@@ -6411,7 +6411,7 @@
         <v>204</v>
       </c>
       <c r="G53" s="160" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
@@ -6434,7 +6434,7 @@
     </row>
     <row r="54" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="216" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C54" s="217"/>
       <c r="D54" s="161">
@@ -6447,7 +6447,7 @@
         <v>204</v>
       </c>
       <c r="G54" s="160" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H54" s="20"/>
       <c r="I54" s="18"/>
@@ -6523,14 +6523,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6789,9 +6789,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6816,11 +6816,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6845,10 +6845,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6871,11 +6871,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6927,11 +6927,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6953,11 +6953,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6984,10 +6984,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7065,14 +7065,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7094,14 +7094,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7132,14 +7132,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7156,22 +7164,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7288,124 +7288,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7434,66 +7434,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7522,66 +7522,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7610,66 +7610,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7698,172 +7698,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7878,25 +7890,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
siga pt 2, documentacion para el posteador pt 1
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE34F8D-E16F-4726-BCD0-6E18F7B1DF4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7DC03C-3EC3-4DFA-B6CF-0F0E489EEFD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="226">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,19 +874,6 @@
     <t>falle muchas veces intentando ver la forma en que poder agregar secciones y variables compatibles con el editor de blogger</t>
   </si>
   <si>
-    <t>resolvi el bug que hacia tener una mala vizualizacion del menu lateral en el editor de blogger, acomode los modulos de forma mas intuitiva, cambie la forma en que se organizan las secciones dentro del main, algo mas intuitivo y previene temblores en el diseño</t>
-  </si>
-  <si>
-    <t>resolver los problema del editor de blogger me tomo mucho, tuve que ver como funcionaban y despues de prueba y error acomode el codigo en parte donde blogger no leyera el display flex, y tambien demore mucho en descubrir como poner dos secciones en la misma fila como lo hise con la seccion principal y lateral en el editor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alinee el header ya que estaba un poco desalineado, a peticion de mi intructor hise la imagen del header mas grande, el cuerpo principal ahora puede ser editado desde el editor de blogger (su separacion dell borde, el borde superior y su color)
-comenze a  realizar la pagina de normarividad, estuve trabajando en la visualizancion de imagenes en estas paginas para que tuvieran una buena principal </t>
-  </si>
-  <si>
-    <t>hoy creo que lo unico que me dio problemas fue quitar esa desalineacion dela imagen del header</t>
-  </si>
-  <si>
     <t>hise que el posicionamiento y el tamaño de la imágenes fuera diferente en las paginas, ademas hise que según el tamaño que se elija es el tamaño que tendran las imágenes, se puede alinear el texto como se desee y tambien se puede separar todo lo que se quiera, si se ponen varia imagenes pequeña juntas se alineean en la misma linea.
 antes cuando la imgen del header no cargaba este se aplastaba, esto ya no va a pasar, ahora su tamaño se conserva aun que la imgen aun no haya cargado</t>
   </si>
@@ -955,6 +942,13 @@
     <t>estuve testeando el posicionamiento manual de ayer, para ver si era facil de usar o si habian errores
 ahora las fotografias o pdfs de un solo caril (cuando no ocupa todo el ancho de la pagina) van a estirarse si su compañero es mas alto que ellos
 hise la pagina de introduccion a siga y siga medio ambiente, estoy empezando a crear el menu de navegacion por sub carpetas</t>
+  </si>
+  <si>
+    <t>hise un prototimo en el que se cambiaba la pagina del blog dentro de siga sin recargar la pagina, luego lo incorpore ala pagina wep, el unico incombeniente esque las 3 paginas estarian en una sola, por lo cual serian dificiles de modificar no tendrian un link individual, asi que descartare esta forma de dividirlas
+alle el error por la cual aveces las imagenes al cargar la pagina dejan de tenes formato y se aplastan, asi que comenze la documentacion del usuario /  posteador del blog con algunas cosas extras, esta documentacion le ire agregando mas cosas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sin duda la forma en que que agregare la diviciones en el menu superior seme ah complicado, por que quiero que sea personalizable </t>
   </si>
 </sst>
 </file>
@@ -2810,6 +2804,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2822,6 +2849,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2873,77 +2939,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2963,99 +3044,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3074,83 +3143,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4137,56 +4131,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4198,45 +4192,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4247,84 +4241,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4333,10 +4327,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4346,8 +4340,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4356,8 +4350,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4366,8 +4360,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4376,8 +4370,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4386,10 +4380,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4400,10 +4394,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4414,8 +4408,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4424,10 +4418,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4438,8 +4432,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4448,8 +4442,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4458,8 +4452,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4468,8 +4462,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4478,8 +4472,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4488,8 +4482,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4498,8 +4492,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4508,8 +4502,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4518,8 +4512,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4528,8 +4522,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4538,10 +4532,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4552,8 +4546,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4562,8 +4556,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4572,8 +4566,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4582,10 +4576,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4596,8 +4590,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4606,10 +4600,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4620,10 +4614,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4634,10 +4628,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4648,8 +4642,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4658,8 +4652,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4668,8 +4662,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4678,8 +4672,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4688,8 +4682,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4698,10 +4692,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4719,6 +4713,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4735,44 +4767,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4788,7 +4782,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4870,14 +4864,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4899,14 +4893,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4928,14 +4922,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4957,14 +4951,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4986,14 +4980,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5189,16 +5183,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5270,20 +5264,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>8</v>
       </c>
-      <c r="F17" s="224" t="s">
-        <v>217</v>
-      </c>
-      <c r="G17" s="225"/>
+      <c r="F17" s="228" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5351,20 +5345,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5406,14 +5400,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5438,17 +5432,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5592,10 +5586,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5622,8 +5616,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5962,7 +5956,7 @@
     </row>
     <row r="40" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="216" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C40" s="217"/>
       <c r="D40" s="161">
@@ -5975,7 +5969,7 @@
         <v>204</v>
       </c>
       <c r="G40" s="160" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
@@ -5998,7 +5992,7 @@
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6011,7 +6005,7 @@
         <v>204</v>
       </c>
       <c r="G41" s="160" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
@@ -6092,7 +6086,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6105,7 +6099,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6128,7 +6122,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6141,7 +6135,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6164,7 +6158,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6177,7 +6171,7 @@
         <v>204</v>
       </c>
       <c r="G46" s="160" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
@@ -6200,7 +6194,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6213,7 +6207,7 @@
         <v>204</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6236,20 +6230,20 @@
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="216" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="C48" s="217"/>
       <c r="D48" s="161">
-        <v>45743</v>
+        <v>45758</v>
       </c>
       <c r="E48" s="161">
-        <v>45743</v>
+        <v>45758</v>
       </c>
       <c r="F48" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6271,22 +6265,12 @@
       <c r="Y48" s="18"/>
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="216" t="s">
-        <v>209</v>
-      </c>
+      <c r="B49" s="216"/>
       <c r="C49" s="217"/>
-      <c r="D49" s="161">
-        <v>45744</v>
-      </c>
-      <c r="E49" s="161">
-        <v>45744</v>
-      </c>
-      <c r="F49" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G49" s="160" t="s">
-        <v>210</v>
-      </c>
+      <c r="D49" s="161"/>
+      <c r="E49" s="161"/>
+      <c r="F49" s="160"/>
+      <c r="G49" s="160"/>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
@@ -6360,7 +6344,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6373,7 +6357,7 @@
         <v>204</v>
       </c>
       <c r="G52" s="160" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H52" s="20"/>
       <c r="I52" s="18"/>
@@ -6396,7 +6380,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
@@ -6409,7 +6393,7 @@
         <v>204</v>
       </c>
       <c r="G53" s="160" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
@@ -6432,7 +6416,7 @@
     </row>
     <row r="54" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="216" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C54" s="217"/>
       <c r="D54" s="161">
@@ -6445,7 +6429,7 @@
         <v>204</v>
       </c>
       <c r="G54" s="160" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H54" s="20"/>
       <c r="I54" s="18"/>
@@ -6521,14 +6505,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6787,9 +6771,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6814,11 +6798,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6843,10 +6827,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6869,11 +6853,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6925,11 +6909,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6951,11 +6935,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6982,10 +6966,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7063,14 +7047,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7092,14 +7076,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7130,14 +7114,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7154,22 +7146,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7286,124 +7270,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7432,66 +7416,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7520,66 +7504,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7608,66 +7592,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7696,172 +7680,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7876,25 +7872,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
siga pt 3, update a la documentacion (imagenes)
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7DC03C-3EC3-4DFA-B6CF-0F0E489EEFD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3B8EA4-56B7-4FE9-952F-F1D2A0F8711A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="217">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -871,53 +871,6 @@
     <t>SI</t>
   </si>
   <si>
-    <t>falle muchas veces intentando ver la forma en que poder agregar secciones y variables compatibles con el editor de blogger</t>
-  </si>
-  <si>
-    <t>hise que el posicionamiento y el tamaño de la imágenes fuera diferente en las paginas, ademas hise que según el tamaño que se elija es el tamaño que tendran las imágenes, se puede alinear el texto como se desee y tambien se puede separar todo lo que se quiera, si se ponen varia imagenes pequeña juntas se alineean en la misma linea.
-antes cuando la imgen del header no cargaba este se aplastaba, esto ya no va a pasar, ahora su tamaño se conserva aun que la imgen aun no haya cargado</t>
-  </si>
-  <si>
-    <t>Las secciones en Blogger funcionan de manera MUY extraña. Los widgets se guardan tanto en Blogger como en el código, por lo que para eliminarlos completamente, hay que hacerlo en ambos lugares.
-Encontrar un equilibrio entre llos estilos de las paginas indibiduales y los post, para que ambos se bean bien alavez que se dejen personalizar y no restrinjan tanto</t>
-  </si>
-  <si>
-    <t>actualize los post a los mas recientes, asi pude ver bug en el posicionamiento y maquilletodo un poco para que todo estuviera mas alineado, tambien cambie los tamaños un poco para que se vea mejor, cambie muchas cosas hacer cade su posiciona miento .
-agrege el menu de navegacion superior, y la pagina e practicas al blog todo responsivo para moviles, aun que cuando tenga mas pagina cambiare cosas de la visualizacion en movil</t>
-  </si>
-  <si>
-    <t>definitivamente el posiscionamieto de las imágenes, tuve que cambiar cosas con mucho cuidado para que no afectara a las paginas del blog, alfinal lo consegui pero definitivamente me costo mucho</t>
-  </si>
-  <si>
-    <t>comenzando el dia estaba tranajando en un herror que hacia que google no quisiera mostrar el boton de abrir en una nueva pestaña, estuve un buen rato regresando actualizaciones donde no me daba ese error de violacion de privacidad pero no pude haya la parte del codigo que lo estaba probocando.
-asi que simplemente puse un texto que abre el pdf en una pestalla nueva para poder descargarla, aprubeche para acomodar un poco mejor los pdfs ademas de corregir otro eror que hacia aparecer un cuadro de dialogo al abrir el pdf (esto estaba en el blog original del sena)
-para finalizar el dia estuve probando diferentes estilos de fondos y jugando con los colores, alfinal lo deje con un fondo de puntos pero me guardare el verde ya que tambien me gusto mucho (no son imagenes, son patrones creados con css, por lo que no reduce la optimizacion)
-comenze en una pagina aparte a hacer un prototipo de un diseño de seleccion de pagina mas moderno y elegante</t>
-  </si>
-  <si>
-    <t>estuve intentando todo lo que seme ocurria para poder mostrar el boton de abrir en una nueva pestaña, luego de un rato vi el origen del problema  que fue una violacion a la pribacidad o condiciones de google, pero nada  cercano del codigo lo afectaba
-con sercano me refiero a estilos o js que afectaran el post, los elimine cambie bla bla y nada, lo que abrio la puerta a que el error debia estar oculto en el resto del codigo, laverdad vi que estaba consumiendo mucho tiempo por que decidi  parar y darle una solucion temporal con los links directo al documento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desde 3/04/2025 hasta 17/04/2025 </t>
-  </si>
-  <si>
-    <t>rediseñe el boton de descarga denuevo, es antiguo no me gustaba tanto asi que quise intentar algo que se viera mas moderno
-tambien remodele la barra de navegacion, con un diseño redondeado y con animaciones de cierre y apertura
-tambien quite el scroll que aparecia antes cuando la pantalla era pequeña ya que era poco estetico, ahora encambio las paginas saltan a la linea de abajo</t>
-  </si>
-  <si>
-    <t>solo fue diseño entonces no tuve ningun problema hoy</t>
-  </si>
-  <si>
-    <t>estuve probando diferentes diseños para que el blog se viera mejor, aun que para poder implementarlos le tendria que preguntar a frankling, vere si los mejoro un poco para ver si los acepta
-ahora cuando pasas el cursor sobre las pagina tienen un diseño un poco mejor, ahora hace enfasis en la pagina que estas y en la pagina a la que quieres ir 
-hise un pequeño diseño para el blog agroturistico del sena, estuve mucho tiempo decidiendo endonde podria ir, y el unico lugar que se me ocurrio fue enciam del buscador</t>
-  </si>
-  <si>
-    <t>nos quedamos sin internet una parte de la tarde</t>
-  </si>
-  <si>
     <t>estuve areglando algo quehacia que el hover de la pagina actual no funcionara bien en las rutas, luego estaba biendo que si se ponia una imagen como baner esta iba a demorar mucho en cargar, entonces como ya habia echo el logo de la pagina decidi intentar crear el baner tambien, lo hise atravez de figma y luego use un codificador para traducirlo como un fonde de css
 me tarde unpoco creando las figuras y posicionandolas de una forma distribuida aunq eu aun asi no me gusta la vercion de escritorio aun que la movil si esta decente, para mejorarla deberia agrandar las figuras en pc</t>
   </si>
@@ -949,6 +902,17 @@
   </si>
   <si>
     <t xml:space="preserve">sin duda la forma en que que agregare la diviciones en el menu superior seme ah complicado, por que quiero que sea personalizable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desde 18/04/2025 hasta 1/06/2025 </t>
+  </si>
+  <si>
+    <t>investigue forma de buscar mas de una etiqueta a la vez, pero aun que funciona, va a ser muy dificil poder meterlo en la interfas y areglar y limpiar las cosas indeseadas que muestra
+agrege nuevas cosas a la documentacion y edite una seccion que ahora permite saber como darle formato a una imagen sin perder calidad
+agrege la pagina de seguridad y salud en el trabajo, ademas de nombres en las paginas, estos nombres quiero tranformarlos en un sistema de categorias editables, pero por ahora tienen esos nombres temporales</t>
+  </si>
+  <si>
+    <t>tuve que ir a una cita medica y areglar unos problemas con mis bitacoras, y afiliacion de riesgo laboral</t>
   </si>
 </sst>
 </file>
@@ -2804,6 +2768,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2837,18 +2894,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2858,85 +2903,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2957,12 +2996,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2975,74 +3008,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3055,96 +3109,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4131,56 +4095,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4192,45 +4156,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4241,84 +4205,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4327,10 +4291,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4340,8 +4304,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4350,8 +4314,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4360,8 +4324,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4370,8 +4334,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4380,10 +4344,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4394,10 +4358,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4408,8 +4372,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4418,10 +4382,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4432,8 +4396,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4442,8 +4406,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4452,8 +4416,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4462,8 +4426,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4472,8 +4436,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4482,8 +4446,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4492,8 +4456,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4502,8 +4466,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4512,8 +4476,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4522,8 +4486,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4532,10 +4496,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4546,8 +4510,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4556,8 +4520,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4566,8 +4530,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4576,10 +4540,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4590,8 +4554,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4600,10 +4564,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4614,10 +4578,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4628,10 +4592,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4642,8 +4606,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4652,8 +4616,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4662,8 +4626,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4672,8 +4636,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4682,8 +4646,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4692,10 +4656,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4713,44 +4677,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4767,6 +4693,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4781,8 +4745,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4864,14 +4828,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4893,14 +4857,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4922,14 +4886,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4951,14 +4915,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4980,14 +4944,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5183,16 +5147,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5264,20 +5228,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
-        <v>8</v>
-      </c>
-      <c r="F17" s="228" t="s">
-        <v>213</v>
-      </c>
-      <c r="G17" s="229"/>
+        <v>9</v>
+      </c>
+      <c r="F17" s="224" t="s">
+        <v>214</v>
+      </c>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5345,20 +5309,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5400,14 +5364,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5432,17 +5396,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5586,10 +5550,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5616,8 +5580,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5955,22 +5919,12 @@
       <c r="Y39" s="18"/>
     </row>
     <row r="40" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="216" t="s">
-        <v>214</v>
-      </c>
+      <c r="B40" s="216"/>
       <c r="C40" s="217"/>
-      <c r="D40" s="161">
-        <v>45750</v>
-      </c>
-      <c r="E40" s="161">
-        <v>45750</v>
-      </c>
-      <c r="F40" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G40" s="160" t="s">
-        <v>215</v>
-      </c>
+      <c r="D40" s="161"/>
+      <c r="E40" s="161"/>
+      <c r="F40" s="160"/>
+      <c r="G40" s="160"/>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
@@ -5991,22 +5945,12 @@
       <c r="Y40" s="18"/>
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="216" t="s">
-        <v>216</v>
-      </c>
+      <c r="B41" s="216"/>
       <c r="C41" s="217"/>
-      <c r="D41" s="161">
-        <v>45751</v>
-      </c>
-      <c r="E41" s="161">
-        <v>45751</v>
-      </c>
-      <c r="F41" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G41" s="160" t="s">
-        <v>217</v>
-      </c>
+      <c r="D41" s="161"/>
+      <c r="E41" s="161"/>
+      <c r="F41" s="160"/>
+      <c r="G41" s="160"/>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
@@ -6030,15 +5974,9 @@
       <c r="B42" s="216"/>
       <c r="C42" s="217"/>
       <c r="D42" s="161"/>
-      <c r="E42" s="161">
-        <v>45737</v>
-      </c>
-      <c r="F42" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G42" s="160" t="s">
-        <v>206</v>
-      </c>
+      <c r="E42" s="161"/>
+      <c r="F42" s="160"/>
+      <c r="G42" s="160"/>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
@@ -6059,12 +5997,22 @@
       <c r="Y42" s="18"/>
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="216"/>
+      <c r="B43" s="216" t="s">
+        <v>215</v>
+      </c>
       <c r="C43" s="217"/>
-      <c r="D43" s="161"/>
-      <c r="E43" s="161"/>
-      <c r="F43" s="160"/>
-      <c r="G43" s="160"/>
+      <c r="D43" s="161">
+        <v>45768</v>
+      </c>
+      <c r="E43" s="161">
+        <v>45768</v>
+      </c>
+      <c r="F43" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G43" s="160" t="s">
+        <v>216</v>
+      </c>
       <c r="H43" s="20"/>
       <c r="I43" s="18"/>
       <c r="J43" s="18"/>
@@ -6086,7 +6034,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6099,7 +6047,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6122,7 +6070,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6135,7 +6083,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6158,7 +6106,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6171,7 +6119,7 @@
         <v>204</v>
       </c>
       <c r="G46" s="160" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
@@ -6194,7 +6142,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6207,7 +6155,7 @@
         <v>204</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6230,7 +6178,7 @@
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="216" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C48" s="217"/>
       <c r="D48" s="161">
@@ -6243,7 +6191,7 @@
         <v>204</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6343,22 +6291,12 @@
       <c r="Y51" s="18"/>
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="216" t="s">
-        <v>207</v>
-      </c>
+      <c r="B52" s="216"/>
       <c r="C52" s="217"/>
-      <c r="D52" s="161">
-        <v>45747</v>
-      </c>
-      <c r="E52" s="161">
-        <v>45747</v>
-      </c>
-      <c r="F52" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G52" s="160" t="s">
-        <v>208</v>
-      </c>
+      <c r="D52" s="161"/>
+      <c r="E52" s="161"/>
+      <c r="F52" s="160"/>
+      <c r="G52" s="160"/>
       <c r="H52" s="20"/>
       <c r="I52" s="18"/>
       <c r="J52" s="18"/>
@@ -6379,22 +6317,12 @@
       <c r="Y52" s="18"/>
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="216" t="s">
-        <v>209</v>
-      </c>
+      <c r="B53" s="216"/>
       <c r="C53" s="217"/>
-      <c r="D53" s="161">
-        <v>45748</v>
-      </c>
-      <c r="E53" s="161">
-        <v>45748</v>
-      </c>
-      <c r="F53" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G53" s="160" t="s">
-        <v>210</v>
-      </c>
+      <c r="D53" s="161"/>
+      <c r="E53" s="161"/>
+      <c r="F53" s="160"/>
+      <c r="G53" s="160"/>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
       <c r="J53" s="18"/>
@@ -6415,22 +6343,12 @@
       <c r="Y53" s="18"/>
     </row>
     <row r="54" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="216" t="s">
-        <v>211</v>
-      </c>
+      <c r="B54" s="216"/>
       <c r="C54" s="217"/>
-      <c r="D54" s="161">
-        <v>45749</v>
-      </c>
-      <c r="E54" s="161">
-        <v>45749</v>
-      </c>
-      <c r="F54" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G54" s="160" t="s">
-        <v>212</v>
-      </c>
+      <c r="D54" s="161"/>
+      <c r="E54" s="161"/>
+      <c r="F54" s="160"/>
+      <c r="G54" s="160"/>
       <c r="H54" s="20"/>
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
@@ -6505,14 +6423,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6771,9 +6689,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6798,11 +6716,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6827,10 +6745,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6853,11 +6771,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6909,11 +6827,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6935,11 +6853,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6966,10 +6884,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7047,14 +6965,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7076,14 +6994,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7114,22 +7032,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7146,14 +7056,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7270,124 +7188,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7416,66 +7334,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7504,66 +7422,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7592,66 +7510,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7680,184 +7598,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7872,13 +7778,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
siga pt 7 animaciones
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBCC2B8-B88B-44F3-9BDE-11B7DEB58FA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3781B9A8-6A5B-4D8D-85B1-8580A44B3BA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="219">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,11 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>estuve testeando el posicionamiento manual de ayer, para ver si era facil de usar o si habian errores
-ahora las fotografias o pdfs de un solo caril (cuando no ocupa todo el ancho de la pagina) van a estirarse si su compañero es mas alto que ellos
-hise la pagina de introduccion a siga y siga medio ambiente, estoy empezando a crear el menu de navegacion por sub carpetas</t>
-  </si>
-  <si>
     <t>hise un prototimo en el que se cambiaba la pagina del blog dentro de siga sin recargar la pagina, luego lo incorpore ala pagina wep, el unico incombeniente esque las 3 paginas estarian en una sola, por lo cual serian dificiles de modificar no tendrian un link individual, asi que descartare esta forma de dividirlas
 alle el error por la cual aveces las imagenes al cargar la pagina dejan de tenes formato y se aplastan, asi que comenze la documentacion del usuario /  posteador del blog con algunas cosas extras, esta documentacion le ire agregando mas cosas</t>
   </si>
@@ -914,6 +909,13 @@
   </si>
   <si>
     <t>estos ultimos dis el progreso ah sido muy lento debido a esta nueva implementacion</t>
+  </si>
+  <si>
+    <t>me dispuse a hacer las animaciones de abrir y cerrar los menus,  me tope con muchos problemas, por que oviamente los menus abiertos deben ocupar mas espacio y animatodo eso seme ah dificultado, ademas que esto debe hacer se con cuidado pues no se me ocurre una forma para que no se salga de patalla,  lo trabaje en un archivo aparte html para ser mas eficiente pero aun asi siento que la mejor solucion sera ponerlo en el menu lateral</t>
+  </si>
+  <si>
+    <t>si el bloque no es tranparente empuja todo el contenido de la pagina para abajo pero si lo es este va a ignorar los limites y simplemente se va a debordar si la pantalla no es lo suficientemete grande
+quiese hacer animaciones compatibles con firefox pero esto me retardo mucho</t>
   </si>
 </sst>
 </file>
@@ -2769,6 +2771,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2802,18 +2897,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2823,85 +2906,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2922,12 +2999,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2940,74 +3011,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3020,96 +3112,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4096,56 +4098,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4157,45 +4159,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4206,84 +4208,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4292,10 +4294,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4305,8 +4307,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4315,8 +4317,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4325,8 +4327,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4335,8 +4337,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4345,10 +4347,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4359,10 +4361,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4373,8 +4375,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4383,10 +4385,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4397,8 +4399,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4407,8 +4409,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4417,8 +4419,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4427,8 +4429,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4437,8 +4439,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4447,8 +4449,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4457,8 +4459,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4467,8 +4469,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4477,8 +4479,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4487,8 +4489,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4497,10 +4499,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4511,8 +4513,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4521,8 +4523,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4531,8 +4533,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4541,10 +4543,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4555,8 +4557,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4565,10 +4567,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4579,10 +4581,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4593,10 +4595,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4607,8 +4609,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4617,8 +4619,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4627,8 +4629,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4637,8 +4639,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4647,8 +4649,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4657,10 +4659,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4678,44 +4680,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4732,6 +4696,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4746,8 +4748,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4829,14 +4831,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4858,14 +4860,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4887,14 +4889,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4916,14 +4918,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4945,14 +4947,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5148,16 +5150,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5229,20 +5231,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>9</v>
       </c>
-      <c r="F17" s="228" t="s">
-        <v>210</v>
-      </c>
-      <c r="G17" s="229"/>
+      <c r="F17" s="224" t="s">
+        <v>209</v>
+      </c>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5310,20 +5312,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5365,14 +5367,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5397,17 +5399,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5551,10 +5553,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5581,8 +5583,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5999,7 +6001,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6012,7 +6014,7 @@
         <v>204</v>
       </c>
       <c r="G43" s="160" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H43" s="20"/>
       <c r="I43" s="18"/>
@@ -6035,7 +6037,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6048,7 +6050,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6071,7 +6073,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6084,7 +6086,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6107,7 +6109,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6143,20 +6145,20 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
-        <v>45757</v>
+        <v>45772</v>
       </c>
       <c r="E47" s="161">
-        <v>45757</v>
+        <v>45772</v>
       </c>
       <c r="F47" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6179,7 +6181,7 @@
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="216" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C48" s="217"/>
       <c r="D48" s="161">
@@ -6192,7 +6194,7 @@
         <v>204</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6424,14 +6426,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6690,9 +6692,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6717,11 +6719,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6746,10 +6748,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6772,11 +6774,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6828,11 +6830,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6854,11 +6856,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6885,10 +6887,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -6966,14 +6968,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -6995,14 +6997,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7033,22 +7035,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7065,14 +7059,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7189,124 +7191,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7335,66 +7337,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7423,66 +7425,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7511,66 +7513,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7599,184 +7601,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7791,13 +7781,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
siga pt 8 superposision  y responsividad
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3781B9A8-6A5B-4D8D-85B1-8580A44B3BA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADA984B-3A75-4884-A7F6-859C9462117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -874,13 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>hise un prototimo en el que se cambiaba la pagina del blog dentro de siga sin recargar la pagina, luego lo incorpore ala pagina wep, el unico incombeniente esque las 3 paginas estarian en una sola, por lo cual serian dificiles de modificar no tendrian un link individual, asi que descartare esta forma de dividirlas
-alle el error por la cual aveces las imagenes al cargar la pagina dejan de tenes formato y se aplastan, asi que comenze la documentacion del usuario /  posteador del blog con algunas cosas extras, esta documentacion le ire agregando mas cosas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sin duda la forma en que que agregare la diviciones en el menu superior seme ah complicado, por que quiero que sea personalizable </t>
-  </si>
-  <si>
     <t xml:space="preserve">Desde 18/04/2025 hasta 1/06/2025 </t>
   </si>
   <si>
@@ -916,6 +909,15 @@
   <si>
     <t>si el bloque no es tranparente empuja todo el contenido de la pagina para abajo pero si lo es este va a ignorar los limites y simplemente se va a debordar si la pantalla no es lo suficientemete grande
 quiese hacer animaciones compatibles con firefox pero esto me retardo mucho</t>
+  </si>
+  <si>
+    <t>hise una vercion del menu desplegable que no empujaba el contenido asi abajo, pero esta no era esponsiva, y el contenido no podia espantirse mas de lo que le permitia el contenedor de arriba
+estuve pensando en si rendirme y solo hacer el menu desplegable en los lateralles ya que ahi no tendria que preocuparme del ancho pos ya seria uno fijo y no dependeria de la posisicon
+estuve revisando algonos desplegables en linea
+alfinal consegui hacer un desplegable que no empuja el contenido, se aplasta si no hay espacio y ademas este puede espandir la caja de el y su padre, esto se puede manipula por ejemplo que solo la expanda cuando se le haga hover, aun que por ahora esta por defecto siempre expandido</t>
+  </si>
+  <si>
+    <t>eh gastado muchos dias en las carpetas del menu</t>
   </si>
 </sst>
 </file>
@@ -2771,6 +2773,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2783,6 +2818,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2834,77 +2908,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2924,99 +3013,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3035,83 +3112,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4098,56 +4100,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4159,45 +4161,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4208,84 +4210,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4294,10 +4296,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4307,8 +4309,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4317,8 +4319,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4327,8 +4329,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4337,8 +4339,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4347,10 +4349,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4361,10 +4363,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4375,8 +4377,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4385,10 +4387,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4399,8 +4401,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4409,8 +4411,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4419,8 +4421,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4429,8 +4431,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4439,8 +4441,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4449,8 +4451,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4459,8 +4461,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4469,8 +4471,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4479,8 +4481,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4489,8 +4491,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4499,10 +4501,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4513,8 +4515,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4523,8 +4525,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4533,8 +4535,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4543,10 +4545,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4557,8 +4559,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4567,10 +4569,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4581,10 +4583,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4595,10 +4597,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4609,8 +4611,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4619,8 +4621,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4629,8 +4631,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4639,8 +4641,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4649,8 +4651,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4659,10 +4661,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4680,6 +4682,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4696,44 +4736,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4749,7 +4751,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4831,14 +4833,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4860,14 +4862,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4889,14 +4891,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4918,14 +4920,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4947,14 +4949,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5150,16 +5152,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5231,20 +5233,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>9</v>
       </c>
-      <c r="F17" s="224" t="s">
-        <v>209</v>
-      </c>
-      <c r="G17" s="225"/>
+      <c r="F17" s="228" t="s">
+        <v>207</v>
+      </c>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5312,20 +5314,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5367,14 +5369,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5399,17 +5401,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5553,10 +5555,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5583,8 +5585,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -6001,7 +6003,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6014,7 +6016,7 @@
         <v>204</v>
       </c>
       <c r="G43" s="160" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H43" s="20"/>
       <c r="I43" s="18"/>
@@ -6037,7 +6039,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6050,7 +6052,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6073,7 +6075,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6086,7 +6088,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6109,7 +6111,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6145,7 +6147,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6158,7 +6160,7 @@
         <v>204</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6180,22 +6182,12 @@
       <c r="Y47" s="18"/>
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="216" t="s">
-        <v>207</v>
-      </c>
+      <c r="B48" s="216"/>
       <c r="C48" s="217"/>
-      <c r="D48" s="161">
-        <v>45758</v>
-      </c>
-      <c r="E48" s="161">
-        <v>45758</v>
-      </c>
-      <c r="F48" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G48" s="160" t="s">
-        <v>208</v>
-      </c>
+      <c r="D48" s="161"/>
+      <c r="E48" s="161"/>
+      <c r="F48" s="160"/>
+      <c r="G48" s="160"/>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
       <c r="J48" s="18"/>
@@ -6242,12 +6234,22 @@
       <c r="Y49" s="18"/>
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="216"/>
+      <c r="B50" s="216" t="s">
+        <v>217</v>
+      </c>
       <c r="C50" s="217"/>
-      <c r="D50" s="161"/>
-      <c r="E50" s="161"/>
-      <c r="F50" s="160"/>
-      <c r="G50" s="160"/>
+      <c r="D50" s="161">
+        <v>45775</v>
+      </c>
+      <c r="E50" s="161">
+        <v>45775</v>
+      </c>
+      <c r="F50" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G50" s="160" t="s">
+        <v>218</v>
+      </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
@@ -6426,14 +6428,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6692,9 +6694,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6719,11 +6721,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6748,10 +6750,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6774,11 +6776,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6830,11 +6832,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6856,11 +6858,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6887,10 +6889,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -6968,14 +6970,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -6997,14 +6999,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7035,14 +7037,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7059,22 +7069,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7191,124 +7193,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7337,66 +7339,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7425,66 +7427,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7513,66 +7515,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7601,172 +7603,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7781,25 +7795,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
siga pt 9 implementacion
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADA984B-3A75-4884-A7F6-859C9462117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F3CC6D-A7CC-4287-BE52-50714EA008B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="221">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -918,6 +918,14 @@
   </si>
   <si>
     <t>eh gastado muchos dias en las carpetas del menu</t>
+  </si>
+  <si>
+    <t>le di algunos retoques a la apariencia y a las animaciones de las carpetas
+luego las emplimente ala pagina finalmente, tambien aprobeche para comentar partes de los estylos para explicar algunas parte importantes, habian muchos conflixtos en los stylos pero finalmente ya tiene una buena aoariencia, las flechas las hise un poco mas anchas y cambian segun el color del texto
+le agrege tambien los links aun que por ahora no tienen la logica para ir a otras paginas pero ya estan puestos</t>
+  </si>
+  <si>
+    <t>algunos estylos causaban que le menu no se habriera corectamente</t>
   </si>
 </sst>
 </file>
@@ -2773,6 +2781,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2806,18 +2907,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2827,85 +2916,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2926,12 +3009,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2944,74 +3021,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3024,96 +3122,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4100,56 +4108,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4161,45 +4169,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4210,84 +4218,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4296,10 +4304,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4309,8 +4317,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4319,8 +4327,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4329,8 +4337,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4339,8 +4347,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4349,10 +4357,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4363,10 +4371,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4377,8 +4385,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4387,10 +4395,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4401,8 +4409,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4411,8 +4419,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4421,8 +4429,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4431,8 +4439,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4441,8 +4449,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4451,8 +4459,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4461,8 +4469,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4471,8 +4479,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4481,8 +4489,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4491,8 +4499,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4501,10 +4509,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4515,8 +4523,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4525,8 +4533,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4535,8 +4543,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4545,10 +4553,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4559,8 +4567,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4569,10 +4577,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4583,10 +4591,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4597,10 +4605,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4611,8 +4619,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4621,8 +4629,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4631,8 +4639,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4641,8 +4649,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4651,8 +4659,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4661,10 +4669,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4682,44 +4690,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4736,6 +4706,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4751,7 +4759,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4833,14 +4841,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4862,14 +4870,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4891,14 +4899,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4920,14 +4928,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4949,14 +4957,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5152,16 +5160,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5233,20 +5241,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>9</v>
       </c>
-      <c r="F17" s="228" t="s">
+      <c r="F17" s="224" t="s">
         <v>207</v>
       </c>
-      <c r="G17" s="229"/>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5314,20 +5322,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5369,14 +5377,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5401,17 +5409,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5555,10 +5563,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5585,8 +5593,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -6270,12 +6278,22 @@
       <c r="Y50" s="18"/>
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="216"/>
+      <c r="B51" s="216" t="s">
+        <v>219</v>
+      </c>
       <c r="C51" s="217"/>
-      <c r="D51" s="161"/>
-      <c r="E51" s="161"/>
-      <c r="F51" s="160"/>
-      <c r="G51" s="160"/>
+      <c r="D51" s="161">
+        <v>45776</v>
+      </c>
+      <c r="E51" s="161">
+        <v>45776</v>
+      </c>
+      <c r="F51" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G51" s="160" t="s">
+        <v>220</v>
+      </c>
       <c r="H51" s="20"/>
       <c r="I51" s="18"/>
       <c r="J51" s="18"/>
@@ -6428,14 +6446,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6694,9 +6712,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6721,11 +6739,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6750,10 +6768,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6776,11 +6794,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6832,11 +6850,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6858,11 +6876,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6889,10 +6907,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -6970,14 +6988,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -6999,14 +7017,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7037,22 +7055,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7069,14 +7079,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7193,124 +7211,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7339,66 +7357,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7427,66 +7445,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7515,66 +7533,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7603,184 +7621,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7795,13 +7801,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
siga pt 10 carpetas con links y funcionales
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F3CC6D-A7CC-4287-BE52-50714EA008B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02D025D-1528-4A4D-B7F4-7DE1A730F0B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="222">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -926,6 +926,10 @@
   </si>
   <si>
     <t>algunos estylos causaban que le menu no se habriera corectamente</t>
+  </si>
+  <si>
+    <t>converti los items de la carpeta en objetos con las propiedades del elemento original, habia un error pues una carpeta al no tener url hasi crashear la pagina y inabilitar todas las funciones debajo de el 
+por ultimo cambien los estylos y puese los links de los elementos de la carpeta, ademas si esta en una pagina de estos items se resaltaran junto a su carpeta padre</t>
   </si>
 </sst>
 </file>
@@ -2781,6 +2785,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2793,6 +2830,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2844,77 +2920,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2934,99 +3025,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3045,83 +3124,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4108,56 +4112,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4169,45 +4173,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4218,84 +4222,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4304,10 +4308,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4317,8 +4321,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4327,8 +4331,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4337,8 +4341,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4347,8 +4351,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4357,10 +4361,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4371,10 +4375,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4385,8 +4389,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4395,10 +4399,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4409,8 +4413,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4419,8 +4423,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4429,8 +4433,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4439,8 +4443,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4449,8 +4453,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4459,8 +4463,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4469,8 +4473,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4479,8 +4483,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4489,8 +4493,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4499,8 +4503,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4509,10 +4513,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4523,8 +4527,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4533,8 +4537,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4543,8 +4547,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4553,10 +4557,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4567,8 +4571,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4577,10 +4581,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4591,10 +4595,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4605,10 +4609,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4619,8 +4623,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4629,8 +4633,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4639,8 +4643,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4649,8 +4653,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4659,8 +4663,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4669,10 +4673,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4690,6 +4694,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4706,44 +4748,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4759,7 +4763,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+      <selection activeCell="B52" sqref="B52:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4841,14 +4845,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4870,14 +4874,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4899,14 +4903,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4928,14 +4932,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4957,14 +4961,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5160,16 +5164,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5241,20 +5245,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>9</v>
       </c>
-      <c r="F17" s="224" t="s">
+      <c r="F17" s="228" t="s">
         <v>207</v>
       </c>
-      <c r="G17" s="225"/>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5322,20 +5326,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5377,14 +5381,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5409,17 +5413,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5563,10 +5567,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5593,8 +5597,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -6314,12 +6318,22 @@
       <c r="Y51" s="18"/>
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="216"/>
+      <c r="B52" s="216" t="s">
+        <v>221</v>
+      </c>
       <c r="C52" s="217"/>
-      <c r="D52" s="161"/>
-      <c r="E52" s="161"/>
-      <c r="F52" s="160"/>
-      <c r="G52" s="160"/>
+      <c r="D52" s="161">
+        <v>45777</v>
+      </c>
+      <c r="E52" s="161">
+        <v>45777</v>
+      </c>
+      <c r="F52" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G52" s="160" t="s">
+        <v>206</v>
+      </c>
       <c r="H52" s="20"/>
       <c r="I52" s="18"/>
       <c r="J52" s="18"/>
@@ -6446,14 +6460,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6712,9 +6726,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6739,11 +6753,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6768,10 +6782,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6794,11 +6808,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6850,11 +6864,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6876,11 +6890,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6907,10 +6921,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -6988,14 +7002,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7017,14 +7031,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7055,14 +7069,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7079,22 +7101,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7211,124 +7225,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7357,66 +7371,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7445,66 +7459,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7533,66 +7547,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7621,172 +7635,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7801,25 +7827,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
notificaciones terminadas y boton de compartir funcional
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768BFFB9-C2C4-4CF1-927B-4321B8716CC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A16D12A-9025-4251-B0C9-6BCB102D9729}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="223">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,14 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>investigue forma de buscar mas de una etiqueta a la vez, pero aun que funciona, va a ser muy dificil poder meterlo en la interfas y areglar y limpiar las cosas indeseadas que muestra
-agrege nuevas cosas a la documentacion y edite una seccion que ahora permite saber como darle formato a una imagen sin perder calidad
-agrege la pagina de seguridad y salud en el trabajo, ademas de nombres en las paginas, estos nombres quiero tranformarlos en un sistema de categorias editables, pero por ahora tienen esos nombres temporales</t>
-  </si>
-  <si>
-    <t>tuve que ir a una cita medica y areglar unos problemas con mis bitacoras, y afiliacion de riesgo laboral</t>
-  </si>
-  <si>
     <t>cree el diseño de como se veran las subcategorias al abrir una carpeta
 logre separar las secciones con &gt; de las demas, esto me tomo mucho tiempo leyendo la documentacion en blogger pero aun no puedo optener una forma de dividirlas y organizarlas por secciones, si lo hisiera por js puro me ahorraria problemas de batallar con las etiquetas de blogger pero si lo hago, al cargar la pagina de morara uno segundos en aparecer las carpetas y eso me gustaria evitarlo</t>
   </si>
@@ -937,6 +929,11 @@
   </si>
   <si>
     <t>tube que ir a una sita con la fisioterapeuta hoy</t>
+  </si>
+  <si>
+    <t>integre las notificaciones a la pagina web y les agrege algunos retoquesmas, por ejemplo que ahora se pueden hacer notificaciones con solo el titulo o solo las descripcion, ahora siempre se tenga un titulo y una descripcion tendra 2 filas, para que tenga 1 debe solo llenar uno de los 2
+cambie un poco el posicionamiento de la imagen del header aun que esta no tiene el titulo del todo centrado tons no se ven bien aun que ya lo haya centrado
+ahora al momento de compartir una publicacion se desplega la interfas para compartir del navegador o en el caso del pc el de windows, adicionalmente si el navegador no es compatible solo copiara la url como lo hacia antes</t>
   </si>
 </sst>
 </file>
@@ -2792,6 +2789,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2825,18 +2915,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2846,85 +2924,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2945,12 +3017,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2963,74 +3029,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3043,96 +3130,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4119,56 +4116,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4180,45 +4177,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4229,84 +4226,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4315,10 +4312,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4328,8 +4325,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4338,8 +4335,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4348,8 +4345,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4358,8 +4355,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4368,10 +4365,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4382,10 +4379,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4396,8 +4393,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4406,10 +4403,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4420,8 +4417,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4430,8 +4427,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4440,8 +4437,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4450,8 +4447,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4460,8 +4457,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4470,8 +4467,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4480,8 +4477,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4490,8 +4487,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4500,8 +4497,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4510,8 +4507,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4520,10 +4517,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4534,8 +4531,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4544,8 +4541,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4554,8 +4551,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4564,10 +4561,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4578,8 +4575,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4588,10 +4585,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4602,10 +4599,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4616,10 +4613,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4630,8 +4627,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4640,8 +4637,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4650,8 +4647,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4660,8 +4657,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4670,8 +4667,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4680,10 +4677,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4701,44 +4698,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4755,6 +4714,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4770,7 +4767,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4852,14 +4849,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4881,14 +4878,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4910,14 +4907,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4939,14 +4936,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4968,14 +4965,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5171,16 +5168,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5252,20 +5249,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>10</v>
       </c>
-      <c r="F17" s="228" t="s">
-        <v>221</v>
-      </c>
-      <c r="G17" s="229"/>
+      <c r="F17" s="224" t="s">
+        <v>219</v>
+      </c>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5333,20 +5330,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5388,14 +5385,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5420,17 +5417,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5574,10 +5571,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5604,8 +5601,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5996,7 +5993,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6009,7 +6006,7 @@
         <v>204</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6032,20 +6029,20 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
-        <v>45768</v>
+        <v>45783</v>
       </c>
       <c r="E43" s="161">
-        <v>45768</v>
+        <v>45783</v>
       </c>
       <c r="F43" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G43" s="160" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H43" s="20"/>
       <c r="I43" s="18"/>
@@ -6068,7 +6065,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6081,7 +6078,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6104,7 +6101,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6117,7 +6114,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6140,7 +6137,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6176,7 +6173,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6189,7 +6186,7 @@
         <v>204</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6264,7 +6261,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6277,7 +6274,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6300,7 +6297,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6313,7 +6310,7 @@
         <v>204</v>
       </c>
       <c r="G51" s="160" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H51" s="20"/>
       <c r="I51" s="18"/>
@@ -6336,7 +6333,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6477,14 +6474,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6743,9 +6740,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6770,11 +6767,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6799,10 +6796,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6825,11 +6822,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6881,11 +6878,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6907,11 +6904,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6938,10 +6935,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7019,14 +7016,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7048,14 +7045,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7086,22 +7083,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7118,14 +7107,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7242,124 +7239,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7388,66 +7385,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7476,66 +7473,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7564,66 +7561,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7652,184 +7649,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7844,13 +7829,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
remake al display flex del body
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A16D12A-9025-4251-B0C9-6BCB102D9729}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3071F4-AC71-462E-AFCE-7EAE61ED0356}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -874,13 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>cree el diseño de como se veran las subcategorias al abrir una carpeta
-logre separar las secciones con &gt; de las demas, esto me tomo mucho tiempo leyendo la documentacion en blogger pero aun no puedo optener una forma de dividirlas y organizarlas por secciones, si lo hisiera por js puro me ahorraria problemas de batallar con las etiquetas de blogger pero si lo hago, al cargar la pagina de morara uno segundos en aparecer las carpetas y eso me gustaria evitarlo</t>
-  </si>
-  <si>
-    <t>la logica en las etiquetas de blogger es limitada y no se puede utilizar funciones normales</t>
-  </si>
-  <si>
     <t>quite una cosa que pintaba la posicision del dedo en movil
 le resto de la mañana estuve leyendo la documentacion de blogger y intentando conseguir idear una forma para manimupular los caracteres individualmente, despues de rato vi una forma de incorpotarlo por js pero la funcion que queriausar ya no era recomentadable usarla, asi que tuve que buscar otra que hisisera eso</t>
   </si>
@@ -934,6 +927,15 @@
     <t>integre las notificaciones a la pagina web y les agrege algunos retoquesmas, por ejemplo que ahora se pueden hacer notificaciones con solo el titulo o solo las descripcion, ahora siempre se tenga un titulo y una descripcion tendra 2 filas, para que tenga 1 debe solo llenar uno de los 2
 cambie un poco el posicionamiento de la imagen del header aun que esta no tiene el titulo del todo centrado tons no se ven bien aun que ya lo haya centrado
 ahora al momento de compartir una publicacion se desplega la interfas para compartir del navegador o en el caso del pc el de windows, adicionalmente si el navegador no es compatible solo copiara la url como lo hacia antes</t>
+  </si>
+  <si>
+    <t>tube que ir a una sita odontologica</t>
+  </si>
+  <si>
+    <t>abia puesto un estilo que hacia que las imagenes en una misma linea no se alinearan automaticamente
+cambie la forma en la que se alinea el cuerpo de una carta permitiendo que cuando hay una fila de varias imagenes en una columna pues el post se adapta a su tamaño 
+removi codigo muerto del esqueleto de carga que tenia antes
+estube probando al final del dia diferentes estilos en la pagina, para ver en que forma se veian mejor posicionados los post, apequeñe un poco el menu derecho en la vercion de pc y redoci su separacion de los bordes en movil</t>
   </si>
 </sst>
 </file>
@@ -2789,6 +2791,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2801,6 +2836,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2852,77 +2926,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2942,99 +3031,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3053,83 +3130,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4116,56 +4118,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4177,45 +4179,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4226,84 +4228,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4312,10 +4314,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4325,8 +4327,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4335,8 +4337,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4345,8 +4347,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4355,8 +4357,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4365,10 +4367,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4379,10 +4381,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4393,8 +4395,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4403,10 +4405,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4417,8 +4419,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4427,8 +4429,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4437,8 +4439,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4447,8 +4449,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4457,8 +4459,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4467,8 +4469,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4477,8 +4479,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4487,8 +4489,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4497,8 +4499,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4507,8 +4509,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4517,10 +4519,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4531,8 +4533,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4541,8 +4543,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4551,8 +4553,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4561,10 +4563,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4575,8 +4577,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4585,10 +4587,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4599,10 +4601,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4613,10 +4615,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4627,8 +4629,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4637,8 +4639,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4647,8 +4649,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4657,8 +4659,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4667,8 +4669,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4677,10 +4679,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4698,6 +4700,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4714,44 +4754,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4767,7 +4769,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="B44" sqref="B44:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4849,14 +4851,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4878,14 +4880,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4907,14 +4909,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4936,14 +4938,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4965,14 +4967,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5168,16 +5170,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5249,20 +5251,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>10</v>
       </c>
-      <c r="F17" s="224" t="s">
-        <v>219</v>
-      </c>
-      <c r="G17" s="225"/>
+      <c r="F17" s="228" t="s">
+        <v>217</v>
+      </c>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5330,20 +5332,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5385,14 +5387,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5417,17 +5419,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5571,10 +5573,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5601,8 +5603,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5993,7 +5995,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6006,7 +6008,7 @@
         <v>204</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6029,7 +6031,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6065,20 +6067,20 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
-        <v>45769</v>
+        <v>45784</v>
       </c>
       <c r="E44" s="161">
-        <v>45769</v>
+        <v>45784</v>
       </c>
       <c r="F44" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6101,7 +6103,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6114,7 +6116,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6137,7 +6139,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6173,7 +6175,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6186,7 +6188,7 @@
         <v>204</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6261,7 +6263,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6274,7 +6276,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6297,7 +6299,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6310,7 +6312,7 @@
         <v>204</v>
       </c>
       <c r="G51" s="160" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H51" s="20"/>
       <c r="I51" s="18"/>
@@ -6333,7 +6335,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6474,14 +6476,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6740,9 +6742,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6767,11 +6769,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6796,10 +6798,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6822,11 +6824,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6878,11 +6880,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6904,11 +6906,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6935,10 +6937,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7016,14 +7018,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7045,14 +7047,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7083,14 +7085,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7107,22 +7117,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7239,124 +7241,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7385,66 +7387,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7473,66 +7475,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7561,66 +7563,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7649,172 +7651,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7829,25 +7843,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
mejora en textos, el codigo ya no  de la funcion de 2 columnas, mejores etiquetas
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3071F4-AC71-462E-AFCE-7EAE61ED0356}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDA163F-B406-4704-A6CA-843DD0138FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="222">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,16 +874,9 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>quite una cosa que pintaba la posicision del dedo en movil
-le resto de la mañana estuve leyendo la documentacion de blogger y intentando conseguir idear una forma para manimupular los caracteres individualmente, despues de rato vi una forma de incorpotarlo por js pero la funcion que queriausar ya no era recomentadable usarla, asi que tuve que buscar otra que hisisera eso</t>
-  </si>
-  <si>
     <t>busque un lugar en el que los script de inicion de la pagina, se ejecutaran ma rapido pero al final vi que no habia diferencia significativas asi que no cambie nada
 cambien la forma de insertar cosas en el html, es mucho mas corta y mas entendible.
 logre separar la informacion por carpetas segun como estes escritas, la posicion de esta se basa en el primer elemente con &gt; que se encuente, oviamente segun el nombre sera u otra carpeta diferente</t>
-  </si>
-  <si>
-    <t>estos ultimos dis el progreso ah sido muy lento debido a esta nueva implementacion</t>
   </si>
   <si>
     <t>me dispuse a hacer las animaciones de abrir y cerrar los menus,  me tope con muchos problemas, por que oviamente los menus abiertos deben ocupar mas espacio y animatodo eso seme ah dificultado, ademas que esto debe hacer se con cuidado pues no se me ocurre una forma para que no se salga de patalla,  lo trabaje en un archivo aparte html para ser mas eficiente pero aun asi siento que la mejor solucion sera ponerlo en el menu lateral</t>
@@ -936,6 +929,15 @@
 cambie la forma en la que se alinea el cuerpo de una carta permitiendo que cuando hay una fila de varias imagenes en una columna pues el post se adapta a su tamaño 
 removi codigo muerto del esqueleto de carga que tenia antes
 estube probando al final del dia diferentes estilos en la pagina, para ver en que forma se veian mejor posicionados los post, apequeñe un poco el menu derecho en la vercion de pc y redoci su separacion de los bordes en movil</t>
+  </si>
+  <si>
+    <t>comenze haciendo pruebas con una entrada de texto, esta antes se centraba indeseablemente, el error era debido a flex que lo centraban
+elimine la funcion que removia los espacios antiguamente, ya que esto de puede hacer desde el editor, simplemente el administrador debe tener cuidado de no dejar saltos de linea al final de la publicacion
+elimine mas codigo que no se usaba
+siguiendo con las publicaciones de texto, cuando una publicacion de texto no es lo suficientemente larga se vulve una tarjeta pequeña, ahora el problema esta en que si esta al lado tiene un publicacion ala lado muy alta esta se estirar hasta tomar su tamaño
+spare 10px mas el titulo del cuerpo de la publicacion y puse mas padding a los lasdos de los post en la vercion de pc para que fueran mas gorditos
+las labels antes se separaban individualmente, lo que hacia que si habian muchas pues se ibas a empujar entre si, ahora es el contenedor que se separa, cuando no hay labels el contenedor desaparece y asi no queda el espacio
+de paso los separe un poco mas de la parte inferior</t>
   </si>
 </sst>
 </file>
@@ -2791,6 +2793,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2824,18 +2919,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2845,85 +2928,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2944,12 +3021,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2962,74 +3033,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3042,96 +3134,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4118,56 +4120,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4179,45 +4181,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4228,84 +4230,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4314,10 +4316,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4327,8 +4329,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4337,8 +4339,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4347,8 +4349,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4357,8 +4359,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4367,10 +4369,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4381,10 +4383,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4395,8 +4397,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4405,10 +4407,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4419,8 +4421,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4429,8 +4431,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4439,8 +4441,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4449,8 +4451,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4459,8 +4461,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4469,8 +4471,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4479,8 +4481,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4489,8 +4491,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4499,8 +4501,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4509,8 +4511,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4519,10 +4521,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4533,8 +4535,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4543,8 +4545,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4553,8 +4555,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4563,10 +4565,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4577,8 +4579,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4587,10 +4589,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4601,10 +4603,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4615,10 +4617,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4629,8 +4631,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4639,8 +4641,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4649,8 +4651,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4659,8 +4661,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4669,8 +4671,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4679,10 +4681,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4700,44 +4702,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4754,6 +4718,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4768,8 +4770,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:C44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4851,14 +4853,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4880,14 +4882,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4909,14 +4911,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4938,14 +4940,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4967,14 +4969,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5170,16 +5172,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5251,20 +5253,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>10</v>
       </c>
-      <c r="F17" s="228" t="s">
-        <v>217</v>
-      </c>
-      <c r="G17" s="229"/>
+      <c r="F17" s="224" t="s">
+        <v>215</v>
+      </c>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5332,20 +5334,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5387,14 +5389,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5419,17 +5421,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5573,10 +5575,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5603,8 +5605,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5995,7 +5997,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6008,7 +6010,7 @@
         <v>204</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6031,7 +6033,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6067,7 +6069,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6080,7 +6082,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6103,20 +6105,20 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
-        <v>45770</v>
+        <v>45785</v>
       </c>
       <c r="E45" s="161">
-        <v>45770</v>
+        <v>45785</v>
       </c>
       <c r="F45" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6139,7 +6141,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6175,7 +6177,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6188,7 +6190,7 @@
         <v>204</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6263,7 +6265,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6276,7 +6278,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6299,7 +6301,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6312,7 +6314,7 @@
         <v>204</v>
       </c>
       <c r="G51" s="160" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H51" s="20"/>
       <c r="I51" s="18"/>
@@ -6335,7 +6337,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6476,14 +6478,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6742,9 +6744,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6769,11 +6771,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6798,10 +6800,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6824,11 +6826,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6880,11 +6882,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6906,11 +6908,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6937,10 +6939,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7018,14 +7020,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7047,14 +7049,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7085,22 +7087,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7117,14 +7111,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7241,124 +7243,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7387,66 +7389,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7475,66 +7477,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7563,66 +7565,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7651,184 +7653,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7843,13 +7833,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
mas compatibilidad con texto, reacomodar espaciados del codigo
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDA163F-B406-4704-A6CA-843DD0138FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BB9E91-2208-45CD-A6A7-AE8F92CA87A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="220">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,18 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>busque un lugar en el que los script de inicion de la pagina, se ejecutaran ma rapido pero al final vi que no habia diferencia significativas asi que no cambie nada
-cambien la forma de insertar cosas en el html, es mucho mas corta y mas entendible.
-logre separar la informacion por carpetas segun como estes escritas, la posicion de esta se basa en el primer elemente con &gt; que se encuente, oviamente segun el nombre sera u otra carpeta diferente</t>
-  </si>
-  <si>
-    <t>me dispuse a hacer las animaciones de abrir y cerrar los menus,  me tope con muchos problemas, por que oviamente los menus abiertos deben ocupar mas espacio y animatodo eso seme ah dificultado, ademas que esto debe hacer se con cuidado pues no se me ocurre una forma para que no se salga de patalla,  lo trabaje en un archivo aparte html para ser mas eficiente pero aun asi siento que la mejor solucion sera ponerlo en el menu lateral</t>
-  </si>
-  <si>
-    <t>si el bloque no es tranparente empuja todo el contenido de la pagina para abajo pero si lo es este va a ignorar los limites y simplemente se va a debordar si la pantalla no es lo suficientemete grande
-quiese hacer animaciones compatibles con firefox pero esto me retardo mucho</t>
-  </si>
-  <si>
     <t>hise una vercion del menu desplegable que no empujaba el contenido asi abajo, pero esta no era esponsiva, y el contenido no podia espantirse mas de lo que le permitia el contenedor de arriba
 estuve pensando en si rendirme y solo hacer el menu desplegable en los lateralles ya que ahi no tendria que preocuparme del ancho pos ya seria uno fijo y no dependeria de la posisicon
 estuve revisando algonos desplegables en linea
@@ -938,6 +926,11 @@
 spare 10px mas el titulo del cuerpo de la publicacion y puse mas padding a los lasdos de los post en la vercion de pc para que fueran mas gorditos
 las labels antes se separaban individualmente, lo que hacia que si habian muchas pues se ibas a empujar entre si, ahora es el contenedor que se separa, cuando no hay labels el contenedor desaparece y asi no queda el espacio
 de paso los separe un poco mas de la parte inferior</t>
+  </si>
+  <si>
+    <t>estuve haciendo una documentacion sobre los errores que hay al copiar un texto, poniendo intrucciones de como quitar el formato. despues de esto me desidi areglar esto cambiando la forma en la que se organizan los bloques de nuevo. despues revise que no hubiera otros errores que probocara mi cambio
+organize de mejor forma los saltos de linea en el codigo, en la evidencia se pueden ver las linea azul  que son las lineas que cambie, pues como elimine espacios inesesarios de la mayoria se ve todo azul
+hise que el header de movil dea mas degado asi se pudier vizualizar el titulo ademas cambie los simbolos sociales de los posts</t>
   </si>
 </sst>
 </file>
@@ -2793,6 +2786,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2805,6 +2831,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2856,77 +2921,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2946,99 +3026,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3057,83 +3125,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4120,56 +4113,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4181,45 +4174,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4230,84 +4223,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4316,10 +4309,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4329,8 +4322,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4339,8 +4332,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4349,8 +4342,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4359,8 +4352,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4369,10 +4362,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4383,10 +4376,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4397,8 +4390,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4407,10 +4400,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4421,8 +4414,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4431,8 +4424,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4441,8 +4434,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4451,8 +4444,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4461,8 +4454,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4471,8 +4464,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4481,8 +4474,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4491,8 +4484,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4501,8 +4494,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4511,8 +4504,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4521,10 +4514,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4535,8 +4528,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4545,8 +4538,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4555,8 +4548,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4565,10 +4558,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4579,8 +4572,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4589,10 +4582,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4603,10 +4596,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4617,10 +4610,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4631,8 +4624,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4641,8 +4634,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4651,8 +4644,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4661,8 +4654,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4671,8 +4664,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4681,10 +4674,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4702,6 +4695,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4718,44 +4749,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4771,7 +4764,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4853,14 +4846,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4882,14 +4875,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4911,14 +4904,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4940,14 +4933,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4969,14 +4962,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5172,16 +5165,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5253,20 +5246,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>10</v>
       </c>
-      <c r="F17" s="224" t="s">
-        <v>215</v>
-      </c>
-      <c r="G17" s="225"/>
+      <c r="F17" s="228" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5334,20 +5327,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5389,14 +5382,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5421,17 +5414,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5575,10 +5568,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5605,8 +5598,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5997,7 +5990,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6010,7 +6003,7 @@
         <v>204</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6033,7 +6026,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6069,7 +6062,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6082,7 +6075,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6105,7 +6098,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6141,14 +6134,14 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
-        <v>45771</v>
+        <v>45786</v>
       </c>
       <c r="E46" s="161">
-        <v>45771</v>
+        <v>45786</v>
       </c>
       <c r="F46" s="160" t="s">
         <v>204</v>
@@ -6176,22 +6169,12 @@
       <c r="Y46" s="18"/>
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="216" t="s">
-        <v>208</v>
-      </c>
+      <c r="B47" s="216"/>
       <c r="C47" s="217"/>
-      <c r="D47" s="161">
-        <v>45772</v>
-      </c>
-      <c r="E47" s="161">
-        <v>45772</v>
-      </c>
-      <c r="F47" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G47" s="160" t="s">
-        <v>209</v>
-      </c>
+      <c r="D47" s="161"/>
+      <c r="E47" s="161"/>
+      <c r="F47" s="160"/>
+      <c r="G47" s="160"/>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
@@ -6265,7 +6248,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6278,7 +6261,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6301,7 +6284,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6314,7 +6297,7 @@
         <v>204</v>
       </c>
       <c r="G51" s="160" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H51" s="20"/>
       <c r="I51" s="18"/>
@@ -6337,7 +6320,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6478,14 +6461,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6744,9 +6727,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6771,11 +6754,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6800,10 +6783,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6826,11 +6809,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6882,11 +6865,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6908,11 +6891,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6939,10 +6922,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7020,14 +7003,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7049,14 +7032,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7087,14 +7070,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7111,22 +7102,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7243,124 +7226,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7389,66 +7372,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7477,66 +7460,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7565,66 +7548,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7653,172 +7636,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7833,25 +7828,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
btn post / comentarios / eliminar codigo
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BB9E91-2208-45CD-A6A7-AE8F92CA87A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD281445-A835-463C-9B22-4ADAF9FD8D4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="222">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -931,6 +931,15 @@
     <t>estuve haciendo una documentacion sobre los errores que hay al copiar un texto, poniendo intrucciones de como quitar el formato. despues de esto me desidi areglar esto cambiando la forma en la que se organizan los bloques de nuevo. despues revise que no hubiera otros errores que probocara mi cambio
 organize de mejor forma los saltos de linea en el codigo, en la evidencia se pueden ver las linea azul  que son las lineas que cambie, pues como elimine espacios inesesarios de la mayoria se ve todo azul
 hise que el header de movil dea mas degado asi se pudier vizualizar el titulo ademas cambie los simbolos sociales de los posts</t>
+  </si>
+  <si>
+    <t>agrege mas espaciado entre el titulo y el cuerpo de un post, los contenedores de los de los botones de interaccion fueron decorados y abarcan mas espacio, adicionamente tienen animaciones al pasar el mause sobre ellos o al oprimirlos
+elimine por completo las antigua funcion de agregar la clase dos columnas, ya que anteriormente le habia quitado la funcionalidad (esto para mas optimizacion y un mejor forma de manejar el tamaño de las imagenes desde el editor de blogger)
+limpie salidas de la consola que usaba para testear la formacion de carpetas
+mejore los comentarios de la funcion de crear carpetas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tube que ir a una radio grafia y no no puede asitir entoda la mañana por los laxantes </t>
   </si>
 </sst>
 </file>
@@ -2786,6 +2795,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2819,18 +2921,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2840,85 +2930,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2939,12 +3023,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2957,74 +3035,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3037,96 +3136,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4113,56 +4122,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4174,45 +4183,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4223,84 +4232,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4309,10 +4318,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4322,8 +4331,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4332,8 +4341,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4342,8 +4351,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4352,8 +4361,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4362,10 +4371,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4376,10 +4385,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4390,8 +4399,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4400,10 +4409,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4414,8 +4423,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4424,8 +4433,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4434,8 +4443,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4444,8 +4453,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4454,8 +4463,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4464,8 +4473,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4474,8 +4483,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4484,8 +4493,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4494,8 +4503,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4504,8 +4513,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4514,10 +4523,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4528,8 +4537,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4538,8 +4547,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4548,8 +4557,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4558,10 +4567,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4572,8 +4581,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4582,10 +4591,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4596,10 +4605,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4610,10 +4619,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4624,8 +4633,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4634,8 +4643,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4644,8 +4653,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4654,8 +4663,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4664,8 +4673,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4674,10 +4683,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4695,44 +4704,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4749,6 +4720,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4763,8 +4772,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4846,14 +4855,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4875,14 +4884,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4904,14 +4913,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4933,14 +4942,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4962,14 +4971,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5165,16 +5174,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5246,20 +5255,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>10</v>
       </c>
-      <c r="F17" s="228" t="s">
+      <c r="F17" s="224" t="s">
         <v>212</v>
       </c>
-      <c r="G17" s="229"/>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5327,20 +5336,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5382,14 +5391,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5414,17 +5423,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5568,10 +5577,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5598,8 +5607,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -6221,12 +6230,22 @@
       <c r="Y48" s="18"/>
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="216"/>
+      <c r="B49" s="216" t="s">
+        <v>220</v>
+      </c>
       <c r="C49" s="217"/>
-      <c r="D49" s="161"/>
-      <c r="E49" s="161"/>
-      <c r="F49" s="160"/>
-      <c r="G49" s="160"/>
+      <c r="D49" s="161">
+        <v>45789</v>
+      </c>
+      <c r="E49" s="161">
+        <v>45789</v>
+      </c>
+      <c r="F49" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G49" s="160" t="s">
+        <v>221</v>
+      </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
@@ -6461,14 +6480,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6727,9 +6746,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6754,11 +6773,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6783,10 +6802,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6809,11 +6828,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6865,11 +6884,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6891,11 +6910,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6922,10 +6941,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7003,14 +7022,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7032,14 +7051,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7070,22 +7089,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7102,14 +7113,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7226,124 +7245,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7372,66 +7391,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7460,66 +7479,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7548,66 +7567,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7636,184 +7655,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7828,13 +7835,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
comentarios / botones de navegacion
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD281445-A835-463C-9B22-4ADAF9FD8D4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250C5812-3E18-4B86-9135-DC07174AFEFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="221">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,23 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>hise una vercion del menu desplegable que no empujaba el contenido asi abajo, pero esta no era esponsiva, y el contenido no podia espantirse mas de lo que le permitia el contenedor de arriba
-estuve pensando en si rendirme y solo hacer el menu desplegable en los lateralles ya que ahi no tendria que preocuparme del ancho pos ya seria uno fijo y no dependeria de la posisicon
-estuve revisando algonos desplegables en linea
-alfinal consegui hacer un desplegable que no empuja el contenido, se aplasta si no hay espacio y ademas este puede espandir la caja de el y su padre, esto se puede manipula por ejemplo que solo la expanda cuando se le haga hover, aun que por ahora esta por defecto siempre expandido</t>
-  </si>
-  <si>
-    <t>eh gastado muchos dias en las carpetas del menu</t>
-  </si>
-  <si>
-    <t>le di algunos retoques a la apariencia y a las animaciones de las carpetas
-luego las emplimente ala pagina finalmente, tambien aprobeche para comentar partes de los estylos para explicar algunas parte importantes, habian muchos conflixtos en los stylos pero finalmente ya tiene una buena aoariencia, las flechas las hise un poco mas anchas y cambian segun el color del texto
-le agrege tambien los links aun que por ahora no tienen la logica para ir a otras paginas pero ya estan puestos</t>
-  </si>
-  <si>
-    <t>algunos estylos causaban que le menu no se habriera corectamente</t>
-  </si>
-  <si>
     <t>converti los items de la carpeta en objetos con las propiedades del elemento original, habia un error pues una carpeta al no tener url hasi crashear la pagina y inabilitar todas las funciones debajo de el 
 por ultimo cambien los estylos y puese los links de los elementos de la carpeta, ademas si esta en una pagina de estos items se resaltaran junto a su carpeta padre</t>
   </si>
@@ -940,6 +923,22 @@
   </si>
   <si>
     <t xml:space="preserve">tube que ir a una radio grafia y no no puede asitir entoda la mañana por los laxantes </t>
+  </si>
+  <si>
+    <t>no encuentr a la forma de poner los comentarios, bueno mas bien areglarlos</t>
+  </si>
+  <si>
+    <t>revisando note que hay un error con las notificaciones en fire fox, pero solo afecta al icono
+descargue el codigo original de la plantilla y comenze a compararlo para mejorar los comentarios (oh almenos dejarlo identico al original)
+re hubique la navegacion entre paginas del post, ademas en el codigo la puse en un lugar mas visible y intuitivo</t>
+  </si>
+  <si>
+    <t>antes el deplegable del menu superior quedaba por debajo de la fecha, le agrege un nivel mas al index
+despues de mover muchas cosas decubri una forma de que la forma de responder vuelva a funcionar, aun que no es una solucion definitiva ya que me gustaria seguir viendo como funcionan los comentario y usar un solucion mas simple de entender
+estaba intentando tambien traer el input para comentar desde la pagina principal para poder opinar sin cambiar de pagina
+despues de un rato mas descubri que puedo solucionar el problema simplemente acomodando en una misma linea una funcion que en el pasado habia desacomodado, problema de los comentarios resuelto
+estuve buscando forma para modificar el html de los comentario pero no encontre nada, la unica forma es cambiando las respuestas a ventanas emergentes, y asi tener control sobre los comentarios pero ir a una pagina diferente a comentar es engorroso y poco practico
+le agrege iconos a lso botones inferiores</t>
   </si>
 </sst>
 </file>
@@ -4772,8 +4771,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5266,7 +5265,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="224" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G17" s="225"/>
       <c r="H17" s="20"/>
@@ -5999,7 +5998,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6012,7 +6011,7 @@
         <v>204</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6035,7 +6034,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6071,7 +6070,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6084,7 +6083,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6107,7 +6106,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6143,7 +6142,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6231,7 +6230,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6244,7 +6243,7 @@
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6267,20 +6266,20 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
-        <v>45775</v>
+        <v>45790</v>
       </c>
       <c r="E50" s="161">
-        <v>45775</v>
+        <v>45790</v>
       </c>
       <c r="F50" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6303,20 +6302,20 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
-        <v>45776</v>
+        <v>45791</v>
       </c>
       <c r="E51" s="161">
-        <v>45776</v>
+        <v>45791</v>
       </c>
       <c r="F51" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G51" s="160" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H51" s="20"/>
       <c r="I51" s="18"/>
@@ -6339,7 +6338,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">

</xml_diff>

<commit_message>
posisionamiento en blogger, burbujas menu left
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250C5812-3E18-4B86-9135-DC07174AFEFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9B230D-6313-4D15-8185-B5E483C0CC39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -874,10 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>converti los items de la carpeta en objetos con las propiedades del elemento original, habia un error pues una carpeta al no tener url hasi crashear la pagina y inabilitar todas las funciones debajo de el 
-por ultimo cambien los estylos y puese los links de los elementos de la carpeta, ademas si esta en una pagina de estos items se resaltaran junto a su carpeta padre</t>
-  </si>
-  <si>
     <t xml:space="preserve">Desde 3/05/2025 hasta 17/05/2025 </t>
   </si>
   <si>
@@ -939,6 +935,12 @@
 despues de un rato mas descubri que puedo solucionar el problema simplemente acomodando en una misma linea una funcion que en el pasado habia desacomodado, problema de los comentarios resuelto
 estuve buscando forma para modificar el html de los comentario pero no encontre nada, la unica forma es cambiando las respuestas a ventanas emergentes, y asi tener control sobre los comentarios pero ir a una pagina diferente a comentar es engorroso y poco practico
 le agrege iconos a lso botones inferiores</t>
+  </si>
+  <si>
+    <t>me dividi un poco en cosas nuevas por implementar, primero un foto de perfil con tu nombre de google, tambien traje de nuevo la barra de busque de blogger donde trae las cosas de cambiar de secion y tu correo pero era un iframe que no podria manipular asique descarte mi idea
+testee un poco el posionamiento en la pagina de blogger ya que un poco inpredecible y aun no descubro como funciona
+depues de leer un rato la documentacion de blogger encontra la forma en la que se posicionan la secciones, se hace atravez de la id #layout y asi se puede afectr el css en bloger sin que cambie la pagina
+comenze a desarrollar una divicion del menu en varias partes, estos son editables desde blogger ademas esta perfectamente acomodados gracias a los que aprendi a la documentacion, cualquiera puede cambiar de lugar tan solo arastrando. un resultado muy satisfactorio</t>
   </si>
 </sst>
 </file>
@@ -2794,6 +2796,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2806,6 +2841,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2857,77 +2931,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2947,99 +3036,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3058,83 +3135,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4121,56 +4123,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4182,45 +4184,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4231,84 +4233,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4317,10 +4319,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4330,8 +4332,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4340,8 +4342,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4350,8 +4352,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4360,8 +4362,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4370,10 +4372,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4384,10 +4386,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4398,8 +4400,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4408,10 +4410,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4422,8 +4424,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4432,8 +4434,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4442,8 +4444,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4452,8 +4454,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4462,8 +4464,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4472,8 +4474,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4482,8 +4484,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4492,8 +4494,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4502,8 +4504,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4512,8 +4514,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4522,10 +4524,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4536,8 +4538,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4546,8 +4548,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4556,8 +4558,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4566,10 +4568,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4580,8 +4582,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4590,10 +4592,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4604,10 +4606,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4618,10 +4620,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4632,8 +4634,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4642,8 +4644,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4652,8 +4654,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4662,8 +4664,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4672,8 +4674,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4682,10 +4684,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4703,6 +4705,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4719,44 +4759,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4772,7 +4774,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4854,14 +4856,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4883,14 +4885,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4912,14 +4914,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4941,14 +4943,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4970,14 +4972,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5173,16 +5175,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5254,20 +5256,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>10</v>
       </c>
-      <c r="F17" s="224" t="s">
-        <v>208</v>
-      </c>
-      <c r="G17" s="225"/>
+      <c r="F17" s="228" t="s">
+        <v>207</v>
+      </c>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5335,20 +5337,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5390,14 +5392,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5422,17 +5424,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5576,10 +5578,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5606,8 +5608,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5998,7 +6000,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6011,7 +6013,7 @@
         <v>204</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6034,7 +6036,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6070,7 +6072,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6083,7 +6085,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6106,7 +6108,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6142,7 +6144,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6230,7 +6232,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6243,7 +6245,7 @@
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6266,7 +6268,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6279,7 +6281,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6302,7 +6304,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6338,14 +6340,14 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
-        <v>45777</v>
+        <v>45792</v>
       </c>
       <c r="E52" s="161">
-        <v>45777</v>
+        <v>45792</v>
       </c>
       <c r="F52" s="160" t="s">
         <v>204</v>
@@ -6479,14 +6481,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6745,9 +6747,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6772,11 +6774,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6801,10 +6803,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6827,11 +6829,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6883,11 +6885,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6909,11 +6911,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6940,10 +6942,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7021,14 +7023,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7050,14 +7052,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7088,14 +7090,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7112,22 +7122,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7244,124 +7246,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7390,66 +7392,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7478,66 +7480,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7566,66 +7568,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7654,172 +7656,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7834,25 +7848,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
buscador mejorado, fecha pegada fixed
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9B230D-6313-4D15-8185-B5E483C0CC39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811079FD-B8F9-4E44-A65A-3613C73C4012}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="222">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -941,6 +941,11 @@
 testee un poco el posionamiento en la pagina de blogger ya que un poco inpredecible y aun no descubro como funciona
 depues de leer un rato la documentacion de blogger encontra la forma en la que se posicionan la secciones, se hace atravez de la id #layout y asi se puede afectr el css en bloger sin que cambie la pagina
 comenze a desarrollar una divicion del menu en varias partes, estos son editables desde blogger ademas esta perfectamente acomodados gracias a los que aprendi a la documentacion, cualquiera puede cambiar de lugar tan solo arastrando. un resultado muy satisfactorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disminui la separacion de de las fechas y correji que no se salieran de su contenedor
+la fecha ahora denuevo vuelve a quedarse anclada ariba al scrolear
+cambien el codigo del buscador y lo hise mas simple, ademas apreovheche para modificar su diseño y el de los textos transitorios, cosa a destacar es que reemplaze la imagen que tenia como lupa por un svg mucho mas liviano </t>
   </si>
 </sst>
 </file>
@@ -2796,6 +2801,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2829,18 +2927,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2850,85 +2936,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2949,12 +3029,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2967,74 +3041,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3047,96 +3142,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4123,56 +4128,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4184,45 +4189,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4233,84 +4238,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4319,10 +4324,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4332,8 +4337,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4342,8 +4347,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4352,8 +4357,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4362,8 +4367,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4372,10 +4377,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4386,10 +4391,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4400,8 +4405,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4410,10 +4415,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4424,8 +4429,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4434,8 +4439,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4444,8 +4449,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4454,8 +4459,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4464,8 +4469,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4474,8 +4479,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4484,8 +4489,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4494,8 +4499,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4504,8 +4509,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4514,8 +4519,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4524,10 +4529,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4538,8 +4543,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4548,8 +4553,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4558,8 +4563,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4568,10 +4573,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4582,8 +4587,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4592,10 +4597,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4606,10 +4611,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4620,10 +4625,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4634,8 +4639,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4644,8 +4649,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4654,8 +4659,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4664,8 +4669,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4674,8 +4679,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4684,10 +4689,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4705,44 +4710,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4759,6 +4726,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4774,7 +4779,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4856,14 +4861,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4885,14 +4890,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4914,14 +4919,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4943,14 +4948,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4972,14 +4977,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5175,16 +5180,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5256,20 +5261,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>10</v>
       </c>
-      <c r="F17" s="228" t="s">
+      <c r="F17" s="224" t="s">
         <v>207</v>
       </c>
-      <c r="G17" s="229"/>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5337,20 +5342,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5392,14 +5397,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5424,17 +5429,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5578,10 +5583,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5608,8 +5613,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -6375,12 +6380,22 @@
       <c r="Y52" s="18"/>
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="216"/>
+      <c r="B53" s="216" t="s">
+        <v>221</v>
+      </c>
       <c r="C53" s="217"/>
-      <c r="D53" s="161"/>
-      <c r="E53" s="161"/>
-      <c r="F53" s="160"/>
-      <c r="G53" s="160"/>
+      <c r="D53" s="161">
+        <v>45793</v>
+      </c>
+      <c r="E53" s="161">
+        <v>45793</v>
+      </c>
+      <c r="F53" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G53" s="160" t="s">
+        <v>206</v>
+      </c>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
       <c r="J53" s="18"/>
@@ -6481,14 +6496,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6747,9 +6762,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6774,11 +6789,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6803,10 +6818,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6829,11 +6844,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6885,11 +6900,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6911,11 +6926,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6942,10 +6957,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7023,14 +7038,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7052,14 +7067,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7090,22 +7105,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7122,14 +7129,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7246,124 +7261,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7392,66 +7407,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7480,66 +7495,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7568,66 +7583,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7656,184 +7671,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7848,13 +7851,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
reorganizacion y footer pt1
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811079FD-B8F9-4E44-A65A-3613C73C4012}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7729C41-B9B0-4ED5-8EDB-45F8C87E917B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="223">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,9 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t xml:space="preserve">Desde 3/05/2025 hasta 17/05/2025 </t>
-  </si>
-  <si>
     <t>segui mejorando el diseño de la notificacion, le agrege un icono según el tipo de etiqueta que sea, todo esto lo hace la funcion y no es necesario especificar el tipo 
 inplemente la imagen que me dio frankling</t>
   </si>
@@ -946,6 +943,15 @@
     <t xml:space="preserve">disminui la separacion de de las fechas y correji que no se salieran de su contenedor
 la fecha ahora denuevo vuelve a quedarse anclada ariba al scrolear
 cambien el codigo del buscador y lo hise mas simple, ademas apreovheche para modificar su diseño y el de los textos transitorios, cosa a destacar es que reemplaze la imagen que tenia como lupa por un svg mucho mas liviano </t>
+  </si>
+  <si>
+    <t>al pasar el cursor sobre e buscador este se ilumina y el mause cambia a pointer, ademas al oprimir este tiene una animacion dando una mejor presentacion
+hay un espacio en blanco al scrolear estoy testeando soluciones como fijar el menu al scrolear y que tenga un scroll independiente, por ahora no me comvense asi que no hare cambios
+pase una parte del tiempo eliminando espaciado inecesario del codigo, y agregar etiquetas  mejores, puse el footer al lugar que es y le di uno detalles para mayor customizacion desde blogger
+prepare el footer, limpie todas las cosas extras y le puse un wiget para poder meterle html dentro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desde 18/05/2025 hasta 01/06/2025 </t>
   </si>
 </sst>
 </file>
@@ -4778,8 +4784,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5269,10 +5275,10 @@
         <v>199</v>
       </c>
       <c r="E17" s="121">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F17" s="224" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="G17" s="225"/>
       <c r="H17" s="20"/>
@@ -5978,12 +5984,22 @@
       <c r="Y40" s="18"/>
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="216"/>
+      <c r="B41" s="216" t="s">
+        <v>221</v>
+      </c>
       <c r="C41" s="217"/>
-      <c r="D41" s="161"/>
-      <c r="E41" s="161"/>
-      <c r="F41" s="160"/>
-      <c r="G41" s="160"/>
+      <c r="D41" s="161">
+        <v>45796</v>
+      </c>
+      <c r="E41" s="161">
+        <v>45796</v>
+      </c>
+      <c r="F41" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G41" s="160" t="s">
+        <v>206</v>
+      </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
@@ -6005,7 +6021,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6018,7 +6034,7 @@
         <v>204</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6041,7 +6057,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6077,7 +6093,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6090,7 +6106,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6113,7 +6129,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6149,7 +6165,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6237,7 +6253,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6250,7 +6266,7 @@
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6273,7 +6289,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6286,7 +6302,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6309,7 +6325,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6345,7 +6361,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6381,7 +6397,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">

</xml_diff>

<commit_message>
footer pt3, optimizacion de iconos
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0708BB-945E-4B0B-93BA-A88676B60509}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5504D4B5-4B30-4422-A597-C8CA597E1D9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -874,11 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>integre las notificaciones a la pagina web y les agrege algunos retoquesmas, por ejemplo que ahora se pueden hacer notificaciones con solo el titulo o solo las descripcion, ahora siempre se tenga un titulo y una descripcion tendra 2 filas, para que tenga 1 debe solo llenar uno de los 2
-cambie un poco el posicionamiento de la imagen del header aun que esta no tiene el titulo del todo centrado tons no se ven bien aun que ya lo haya centrado
-ahora al momento de compartir una publicacion se desplega la interfas para compartir del navegador o en el caso del pc el de windows, adicionalmente si el navegador no es compatible solo copiara la url como lo hacia antes</t>
-  </si>
-  <si>
     <t>tube que ir a una sita odontologica</t>
   </si>
   <si>
@@ -950,6 +945,12 @@
     <t>probe algunos diseos nuevos para el blog, viencule algunas cosas al editor de blogger  para mas personalizacion
 organize la navegacion con comentarios, para mas eficiencia y encontrar las cosas con mayor facilidad
 hise el maquetado  del footer ya lo complete, ahora falta reponsividad y agregarlo a la pagina principal</t>
+  </si>
+  <si>
+    <t>cambie la forma en que se posionaban las cosas por dentro para poder cambiar los temas una una mejor manera, cree un tema claro y oscuro para que mi frankling eligiera uno
+luego de unos detalles extras agregados al tema oscuro, lo hise reponsivo para dispositivos moviles y lo implemente a la pagina
+borre algunas cosas de los estylos de la pagina ya que me daba conflicto co mis cosas
+reduje el tamaño del logo de intagram de 8k de caracteres a 4k, hise lo mismo con los demas que era mas livianos, como de 1k a 0.5k y asi</t>
   </si>
 </sst>
 </file>
@@ -2805,6 +2806,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2838,18 +2932,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2859,85 +2941,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2958,12 +3034,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2976,74 +3046,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3056,96 +3147,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4132,56 +4133,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4193,45 +4194,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4242,84 +4243,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4328,10 +4329,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4341,8 +4342,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4351,8 +4352,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4361,8 +4362,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4371,8 +4372,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4381,10 +4382,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4395,10 +4396,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4409,8 +4410,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4419,10 +4420,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4433,8 +4434,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4443,8 +4444,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4453,8 +4454,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4463,8 +4464,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4473,8 +4474,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4483,8 +4484,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4493,8 +4494,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4503,8 +4504,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4513,8 +4514,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4523,8 +4524,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4533,10 +4534,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4547,8 +4548,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4557,8 +4558,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4567,8 +4568,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4577,10 +4578,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4591,8 +4592,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4601,10 +4602,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4615,10 +4616,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4629,10 +4630,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4643,8 +4644,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4653,8 +4654,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4663,8 +4664,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4673,8 +4674,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4683,8 +4684,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4693,10 +4694,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4714,44 +4715,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4768,6 +4731,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4865,14 +4866,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4894,14 +4895,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4923,14 +4924,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4952,14 +4953,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4981,14 +4982,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5184,16 +5185,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5265,20 +5266,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>11</v>
       </c>
-      <c r="F17" s="228" t="s">
-        <v>220</v>
-      </c>
-      <c r="G17" s="229"/>
+      <c r="F17" s="224" t="s">
+        <v>219</v>
+      </c>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5346,20 +5347,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5401,14 +5402,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5433,17 +5434,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5587,10 +5588,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5617,8 +5618,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5983,7 +5984,7 @@
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6019,7 +6020,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6055,14 +6056,14 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
-        <v>45783</v>
+        <v>45798</v>
       </c>
       <c r="E43" s="161">
-        <v>45783</v>
+        <v>45798</v>
       </c>
       <c r="F43" s="160" t="s">
         <v>204</v>
@@ -6091,7 +6092,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6104,7 +6105,7 @@
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6127,7 +6128,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6163,7 +6164,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6251,7 +6252,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6264,7 +6265,7 @@
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6287,7 +6288,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6300,7 +6301,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6323,7 +6324,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6359,7 +6360,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6395,7 +6396,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
@@ -6510,14 +6511,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6776,9 +6777,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6803,11 +6804,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6832,10 +6833,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6858,11 +6859,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6914,11 +6915,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6940,11 +6941,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6971,10 +6972,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7052,14 +7053,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7081,14 +7082,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7119,22 +7120,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7151,14 +7144,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7275,124 +7276,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7421,66 +7422,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7509,66 +7510,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7597,66 +7598,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7685,184 +7686,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7877,13 +7866,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
footer pt FINAl, paginacion btn pt1
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5504D4B5-4B30-4422-A597-C8CA597E1D9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349AC00B-36A7-4079-B25A-718CEF22F0FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="221">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,15 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>tube que ir a una sita odontologica</t>
-  </si>
-  <si>
-    <t>abia puesto un estilo que hacia que las imagenes en una misma linea no se alinearan automaticamente
-cambie la forma en la que se alinea el cuerpo de una carta permitiendo que cuando hay una fila de varias imagenes en una columna pues el post se adapta a su tamaño 
-removi codigo muerto del esqueleto de carga que tenia antes
-estube probando al final del dia diferentes estilos en la pagina, para ver en que forma se veian mejor posicionados los post, apequeñe un poco el menu derecho en la vercion de pc y redoci su separacion de los bordes en movil</t>
-  </si>
-  <si>
     <t>comenze haciendo pruebas con una entrada de texto, esta antes se centraba indeseablemente, el error era debido a flex que lo centraban
 elimine la funcion que removia los espacios antiguamente, ya que esto de puede hacer desde el editor, simplemente el administrador debe tener cuidado de no dejar saltos de linea al final de la publicacion
 elimine mas codigo que no se usaba
@@ -951,6 +942,13 @@
 luego de unos detalles extras agregados al tema oscuro, lo hise reponsivo para dispositivos moviles y lo implemente a la pagina
 borre algunas cosas de los estylos de la pagina ya que me daba conflicto co mis cosas
 reduje el tamaño del logo de intagram de 8k de caracteres a 4k, hise lo mismo con los demas que era mas livianos, como de 1k a 0.5k y asi</t>
+  </si>
+  <si>
+    <t>queria reducir el tamaño del logo de insta pues pesaba mucho, asi que lo coloree yo mismo (busque como funcionan los svg) y hise un coloreado mas simple con menos detalles pequeños pero bastante parecido al original
+aregle detalles de la mayoria, ya que algunos era dificil de ponerles color y esas cosas
+agrege todas las redes oficiales al footer junto asus respectivos diseños y animaciones, con esto concluyo el footer
+el borde gris que rodea el blog desaparece cuando la pantalla se vulve mas pequeña
+decore y mejore los botone de pasar de pagina, soma mas grandes y tienen animaciones al oprimirlos</t>
   </si>
 </sst>
 </file>
@@ -2806,6 +2804,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2818,6 +2849,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2869,77 +2939,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2959,99 +3044,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3070,83 +3143,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4133,56 +4131,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4194,45 +4192,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4243,84 +4241,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4329,10 +4327,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4342,8 +4340,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4352,8 +4350,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4362,8 +4360,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4372,8 +4370,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4382,10 +4380,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4396,10 +4394,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4410,8 +4408,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4420,10 +4418,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4434,8 +4432,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4444,8 +4442,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4454,8 +4452,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4464,8 +4462,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4474,8 +4472,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4484,8 +4482,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4494,8 +4492,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4504,8 +4502,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4514,8 +4512,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4524,8 +4522,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4534,10 +4532,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4548,8 +4546,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4558,8 +4556,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4568,8 +4566,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4578,10 +4576,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4592,8 +4590,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4602,10 +4600,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4616,10 +4614,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4630,10 +4628,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4644,8 +4642,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4654,8 +4652,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4664,8 +4662,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4674,8 +4672,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4684,8 +4682,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4694,10 +4692,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4715,6 +4713,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4731,44 +4767,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4784,7 +4782,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,14 +4864,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4895,14 +4893,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4924,14 +4922,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4953,14 +4951,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4982,14 +4980,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5185,16 +5183,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5266,20 +5264,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>11</v>
       </c>
-      <c r="F17" s="224" t="s">
-        <v>219</v>
-      </c>
-      <c r="G17" s="225"/>
+      <c r="F17" s="228" t="s">
+        <v>217</v>
+      </c>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5347,20 +5345,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5402,14 +5400,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5434,17 +5432,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5588,10 +5586,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5618,8 +5616,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5984,7 +5982,7 @@
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6020,7 +6018,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6056,7 +6054,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6092,20 +6090,20 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
-        <v>45784</v>
+        <v>45799</v>
       </c>
       <c r="E44" s="161">
-        <v>45784</v>
+        <v>45799</v>
       </c>
       <c r="F44" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G44" s="160" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6128,7 +6126,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6164,7 +6162,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6252,7 +6250,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6265,7 +6263,7 @@
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6288,7 +6286,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6301,7 +6299,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6324,7 +6322,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6360,7 +6358,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6396,7 +6394,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
@@ -6511,14 +6509,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6777,9 +6775,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6804,11 +6802,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6833,10 +6831,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6859,11 +6857,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6915,11 +6913,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6941,11 +6939,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6972,10 +6970,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7053,14 +7051,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7082,14 +7080,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7120,14 +7118,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7144,22 +7150,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7276,124 +7274,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7422,66 +7420,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7510,66 +7508,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7598,66 +7596,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7686,172 +7684,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7866,25 +7876,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
paginacion btn pt2, agregar enlases pt1
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349AC00B-36A7-4079-B25A-718CEF22F0FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41277247-1E0E-4BE4-9F10-8F2C66911275}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="222">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,15 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>comenze haciendo pruebas con una entrada de texto, esta antes se centraba indeseablemente, el error era debido a flex que lo centraban
-elimine la funcion que removia los espacios antiguamente, ya que esto de puede hacer desde el editor, simplemente el administrador debe tener cuidado de no dejar saltos de linea al final de la publicacion
-elimine mas codigo que no se usaba
-siguiendo con las publicaciones de texto, cuando una publicacion de texto no es lo suficientemente larga se vulve una tarjeta pequeña, ahora el problema esta en que si esta al lado tiene un publicacion ala lado muy alta esta se estirar hasta tomar su tamaño
-spare 10px mas el titulo del cuerpo de la publicacion y puse mas padding a los lasdos de los post en la vercion de pc para que fueran mas gorditos
-las labels antes se separaban individualmente, lo que hacia que si habian muchas pues se ibas a empujar entre si, ahora es el contenedor que se separa, cuando no hay labels el contenedor desaparece y asi no queda el espacio
-de paso los separe un poco mas de la parte inferior</t>
-  </si>
-  <si>
     <t>estuve haciendo una documentacion sobre los errores que hay al copiar un texto, poniendo intrucciones de como quitar el formato. despues de esto me desidi areglar esto cambiando la forma en la que se organizan los bloques de nuevo. despues revise que no hubiera otros errores que probocara mi cambio
 organize de mejor forma los saltos de linea en el codigo, en la evidencia se pueden ver las linea azul  que son las lineas que cambie, pues como elimine espacios inesesarios de la mayoria se ve todo azul
 hise que el header de movil dea mas degado asi se pudier vizualizar el titulo ademas cambie los simbolos sociales de los posts</t>
@@ -949,6 +940,17 @@
 agrege todas las redes oficiales al footer junto asus respectivos diseños y animaciones, con esto concluyo el footer
 el borde gris que rodea el blog desaparece cuando la pantalla se vulve mas pequeña
 decore y mejore los botone de pasar de pagina, soma mas grandes y tienen animaciones al oprimirlos</t>
+  </si>
+  <si>
+    <t>comenze haciendo pruebas con una entrada de texto, esta antes se centraba indeseablemente, el error era debido a flex que lo centraban
+elimine la funcion que removia los espacios antiguamente, ya que en vez que los botones desaparescan, hise un diseño que se pusiera cuando estan inactivos, agrege que al estar en el menu no se pueda oprimir este mismo
+hable con franklin un rato y hiseun diseño en el que el menu izquierdo queda fijo mientras se scrolean las publicaciones
+los comentarios ya no se pegan al borde cuando esve en una vista de movil
+comenze pasar y anotarme paginas externas que tiene el blog, y limpio un poco el codigo que extraje de la wep original ya que habian muchas cosas redundantes... asi almenos era mas facil de leer el codigo
+de paso los separe un poco mas de la parte inferior</t>
+  </si>
+  <si>
+    <t>la mitad de la mañana hubo un evento de la inglesia, ademas de eso nada mas</t>
   </si>
 </sst>
 </file>
@@ -2804,6 +2806,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2837,18 +2932,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2858,85 +2941,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2957,12 +3034,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2975,74 +3046,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3055,96 +3147,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4131,56 +4133,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4192,45 +4194,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4241,84 +4243,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4327,10 +4329,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4340,8 +4342,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4350,8 +4352,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4360,8 +4362,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4370,8 +4372,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4380,10 +4382,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4394,10 +4396,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4408,8 +4410,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4418,10 +4420,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4432,8 +4434,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4442,8 +4444,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4452,8 +4454,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4462,8 +4464,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4472,8 +4474,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4482,8 +4484,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4492,8 +4494,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4502,8 +4504,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4512,8 +4514,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4522,8 +4524,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4532,10 +4534,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4546,8 +4548,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4556,8 +4558,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4566,8 +4568,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4576,10 +4578,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4590,8 +4592,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4600,10 +4602,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4614,10 +4616,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4628,10 +4630,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4642,8 +4644,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4652,8 +4654,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4662,8 +4664,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4672,8 +4674,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4682,8 +4684,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4692,10 +4694,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4713,44 +4715,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4767,6 +4731,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4782,7 +4784,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4864,14 +4866,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4893,14 +4895,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4922,14 +4924,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4951,14 +4953,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4980,14 +4982,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5183,16 +5185,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5264,20 +5266,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>11</v>
       </c>
-      <c r="F17" s="228" t="s">
-        <v>217</v>
-      </c>
-      <c r="G17" s="229"/>
+      <c r="F17" s="224" t="s">
+        <v>216</v>
+      </c>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5345,20 +5347,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5400,14 +5402,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5432,17 +5434,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5586,10 +5588,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5616,8 +5618,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5982,7 +5984,7 @@
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6018,7 +6020,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6054,7 +6056,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6090,7 +6092,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6126,20 +6128,20 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
-        <v>45785</v>
+        <v>45800</v>
       </c>
       <c r="E45" s="161">
-        <v>45785</v>
+        <v>45800</v>
       </c>
       <c r="F45" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6162,7 +6164,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6250,7 +6252,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6263,7 +6265,7 @@
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6286,7 +6288,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6299,7 +6301,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6322,7 +6324,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6358,7 +6360,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6394,7 +6396,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
@@ -6509,14 +6511,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6775,9 +6777,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6802,11 +6804,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6831,10 +6833,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6857,11 +6859,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6913,11 +6915,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6939,11 +6941,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6970,10 +6972,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7051,14 +7053,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7080,14 +7082,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7118,22 +7120,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7150,14 +7144,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7274,124 +7276,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7420,66 +7422,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7508,66 +7510,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7596,66 +7598,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7684,184 +7686,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7876,13 +7866,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
actualizacion de menu lateral
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41277247-1E0E-4BE4-9F10-8F2C66911275}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F698F9-4A62-4797-B433-98847D0CDDF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -874,11 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>estuve haciendo una documentacion sobre los errores que hay al copiar un texto, poniendo intrucciones de como quitar el formato. despues de esto me desidi areglar esto cambiando la forma en la que se organizan los bloques de nuevo. despues revise que no hubiera otros errores que probocara mi cambio
-organize de mejor forma los saltos de linea en el codigo, en la evidencia se pueden ver las linea azul  que son las lineas que cambie, pues como elimine espacios inesesarios de la mayoria se ve todo azul
-hise que el header de movil dea mas degado asi se pudier vizualizar el titulo ademas cambie los simbolos sociales de los posts</t>
-  </si>
-  <si>
     <t>agrege mas espaciado entre el titulo y el cuerpo de un post, los contenedores de los de los botones de interaccion fueron decorados y abarcan mas espacio, adicionamente tienen animaciones al pasar el mause sobre ellos o al oprimirlos
 elimine por completo las antigua funcion de agregar la clase dos columnas, ya que anteriormente le habia quitado la funcionalidad (esto para mas optimizacion y un mejor forma de manejar el tamaño de las imagenes desde el editor de blogger)
 limpie salidas de la consola que usaba para testear la formacion de carpetas
@@ -951,6 +946,11 @@
   </si>
   <si>
     <t>la mitad de la mañana hubo un evento de la inglesia, ademas de eso nada mas</t>
+  </si>
+  <si>
+    <t>hise un nuevo diseño para las paginas que se agregen al lateral, ahora se ve menos vacio todo, divi di los links en 2 categorias servicios que el sena ofrese al publico y servicios que afrese a los aprendises
+estuve revisando la pagina del sena y recatando todos los links que aun servian, revise y ya no queda ningun link por agregar
+reorganize las secciones del menu y ahora al scrolear el historial se queda anclar</t>
   </si>
 </sst>
 </file>
@@ -2806,6 +2806,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2818,6 +2851,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2869,77 +2941,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2959,99 +3046,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3070,83 +3145,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4133,56 +4133,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4194,45 +4194,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4243,84 +4243,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4329,10 +4329,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4342,8 +4342,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4352,8 +4352,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4362,8 +4362,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4372,8 +4372,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4382,10 +4382,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4396,10 +4396,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4410,8 +4410,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4420,10 +4420,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4434,8 +4434,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4444,8 +4444,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4454,8 +4454,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4464,8 +4464,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4474,8 +4474,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4484,8 +4484,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4494,8 +4494,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4504,8 +4504,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4514,8 +4514,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4524,8 +4524,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4534,10 +4534,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4548,8 +4548,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4558,8 +4558,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4568,8 +4568,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4578,10 +4578,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4592,8 +4592,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4602,10 +4602,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4616,10 +4616,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4630,10 +4630,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4644,8 +4644,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4654,8 +4654,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4664,8 +4664,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4674,8 +4674,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4684,8 +4684,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4694,10 +4694,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4715,6 +4715,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4731,44 +4769,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4783,8 +4783,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,14 +4866,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4895,14 +4895,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4924,14 +4924,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4953,14 +4953,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4982,14 +4982,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5185,16 +5185,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5266,20 +5266,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>11</v>
       </c>
-      <c r="F17" s="224" t="s">
-        <v>216</v>
-      </c>
-      <c r="G17" s="225"/>
+      <c r="F17" s="228" t="s">
+        <v>215</v>
+      </c>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5347,20 +5347,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5402,14 +5402,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5434,17 +5434,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5588,10 +5588,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5618,8 +5618,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5984,7 +5984,7 @@
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6020,7 +6020,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6056,7 +6056,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6092,7 +6092,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6128,7 +6128,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6141,7 +6141,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6163,22 +6163,12 @@
       <c r="Y45" s="18"/>
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="216" t="s">
-        <v>207</v>
-      </c>
+      <c r="B46" s="216"/>
       <c r="C46" s="217"/>
-      <c r="D46" s="161">
-        <v>45786</v>
-      </c>
-      <c r="E46" s="161">
-        <v>45786</v>
-      </c>
-      <c r="F46" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G46" s="160" t="s">
-        <v>206</v>
-      </c>
+      <c r="D46" s="161"/>
+      <c r="E46" s="161"/>
+      <c r="F46" s="160"/>
+      <c r="G46" s="160"/>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
@@ -6225,12 +6215,22 @@
       <c r="Y47" s="18"/>
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="216"/>
+      <c r="B48" s="216" t="s">
+        <v>221</v>
+      </c>
       <c r="C48" s="217"/>
-      <c r="D48" s="161"/>
-      <c r="E48" s="161"/>
-      <c r="F48" s="160"/>
-      <c r="G48" s="160"/>
+      <c r="D48" s="161">
+        <v>45800</v>
+      </c>
+      <c r="E48" s="161">
+        <v>45800</v>
+      </c>
+      <c r="F48" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="G48" s="160" t="s">
+        <v>206</v>
+      </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
       <c r="J48" s="18"/>
@@ -6252,7 +6252,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6265,7 +6265,7 @@
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6288,7 +6288,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6301,7 +6301,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6324,7 +6324,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6360,7 +6360,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6396,7 +6396,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
@@ -6511,14 +6511,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6777,9 +6777,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6804,11 +6804,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6833,10 +6833,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6859,11 +6859,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6915,11 +6915,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6941,11 +6941,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6972,10 +6972,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7053,14 +7053,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7082,14 +7082,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7120,14 +7120,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7144,22 +7152,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7276,124 +7276,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7422,66 +7422,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7510,66 +7510,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7598,66 +7598,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7686,172 +7686,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7866,25 +7878,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
menu inferior pt1, imagen
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F698F9-4A62-4797-B433-98847D0CDDF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB5E79F-5E15-476B-AF84-BDE8EF5225B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="221">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -874,15 +874,6 @@
     <t>sin dificultades</t>
   </si>
   <si>
-    <t>agrege mas espaciado entre el titulo y el cuerpo de un post, los contenedores de los de los botones de interaccion fueron decorados y abarcan mas espacio, adicionamente tienen animaciones al pasar el mause sobre ellos o al oprimirlos
-elimine por completo las antigua funcion de agregar la clase dos columnas, ya que anteriormente le habia quitado la funcionalidad (esto para mas optimizacion y un mejor forma de manejar el tamaño de las imagenes desde el editor de blogger)
-limpie salidas de la consola que usaba para testear la formacion de carpetas
-mejore los comentarios de la funcion de crear carpetas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tube que ir a una radio grafia y no no puede asitir entoda la mañana por los laxantes </t>
-  </si>
-  <si>
     <t>no encuentr a la forma de poner los comentarios, bueno mas bien areglarlos</t>
   </si>
   <si>
@@ -951,6 +942,13 @@
     <t>hise un nuevo diseño para las paginas que se agregen al lateral, ahora se ve menos vacio todo, divi di los links en 2 categorias servicios que el sena ofrese al publico y servicios que afrese a los aprendises
 estuve revisando la pagina del sena y recatando todos los links que aun servian, revise y ya no queda ningun link por agregar
 reorganize las secciones del menu y ahora al scrolear el historial se queda anclar</t>
+  </si>
+  <si>
+    <t>nuevo widget, es una imagen que estaba en el anterior blog del sena, solo que busque a fuente original y esta tiene mejor resolucion, ademas la comprimi para que ocupara menos
+comenxe a a subir css de los widgets a rruba, asi tener el css en un mismo lugar adema que ahia carga mas rapido que abajo
+cree un boton para desplegar el menu cuando este se plega, estube probando varios diseños y ese fue el que mas me gusto
+quise no agregar solo ese boton si no que agregar un menu de navegacion que sirva tanto para subir y bajar del todo de la pagina
+esto por que frankling lo tomo como un problema por que la pagina es muy larga</t>
   </si>
 </sst>
 </file>
@@ -2806,6 +2804,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2839,18 +2930,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2860,85 +2939,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2959,12 +3032,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2977,74 +3044,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3057,96 +3145,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4133,56 +4131,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4194,45 +4192,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4243,84 +4241,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4329,10 +4327,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4342,8 +4340,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4352,8 +4350,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4362,8 +4360,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4372,8 +4370,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4382,10 +4380,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4396,10 +4394,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4410,8 +4408,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4420,10 +4418,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4434,8 +4432,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4444,8 +4442,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4454,8 +4452,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4464,8 +4462,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4474,8 +4472,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4484,8 +4482,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4494,8 +4492,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4504,8 +4502,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4514,8 +4512,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4524,8 +4522,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4534,10 +4532,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4548,8 +4546,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4558,8 +4556,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4568,8 +4566,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4578,10 +4576,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4592,8 +4590,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4602,10 +4600,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4616,10 +4614,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4630,10 +4628,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4644,8 +4642,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4654,8 +4652,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4664,8 +4662,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4674,8 +4672,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4684,8 +4682,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4694,10 +4692,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4715,44 +4713,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4769,6 +4729,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4783,8 +4781,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48:C48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,14 +4864,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4895,14 +4893,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4924,14 +4922,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4953,14 +4951,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4982,14 +4980,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5185,16 +5183,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5266,20 +5264,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>11</v>
       </c>
-      <c r="F17" s="228" t="s">
-        <v>215</v>
-      </c>
-      <c r="G17" s="229"/>
+      <c r="F17" s="224" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5347,20 +5345,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>200</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5402,14 +5400,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5434,17 +5432,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5588,10 +5586,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5618,8 +5616,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5984,7 +5982,7 @@
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6020,7 +6018,7 @@
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6056,7 +6054,7 @@
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="216" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C43" s="217"/>
       <c r="D43" s="161">
@@ -6092,7 +6090,7 @@
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6128,7 +6126,7 @@
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="216" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C45" s="217"/>
       <c r="D45" s="161">
@@ -6141,7 +6139,7 @@
         <v>204</v>
       </c>
       <c r="G45" s="160" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
@@ -6216,14 +6214,14 @@
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="216" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C48" s="217"/>
       <c r="D48" s="161">
-        <v>45800</v>
+        <v>45803</v>
       </c>
       <c r="E48" s="161">
-        <v>45800</v>
+        <v>45803</v>
       </c>
       <c r="F48" s="160" t="s">
         <v>204</v>
@@ -6252,20 +6250,20 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
-        <v>45789</v>
+        <v>45804</v>
       </c>
       <c r="E49" s="161">
-        <v>45789</v>
+        <v>45804</v>
       </c>
       <c r="F49" s="160" t="s">
         <v>204</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6288,7 +6286,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6301,7 +6299,7 @@
         <v>204</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6324,7 +6322,7 @@
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
@@ -6360,7 +6358,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6396,7 +6394,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
@@ -6511,14 +6509,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6777,9 +6775,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6804,11 +6802,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6833,10 +6831,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6859,11 +6857,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6915,11 +6913,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6941,11 +6939,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6972,10 +6970,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7053,14 +7051,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7082,14 +7080,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7120,22 +7118,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7152,14 +7142,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7276,124 +7274,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
      